<commit_message>
nieuwenhuys xls upodated with tranverse and coronal plan + both side
</commit_message>
<xml_diff>
--- a/Data/jointPatterns/Nieuwenhuys2017.xlsx
+++ b/Data/jointPatterns/Nieuwenhuys2017.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="72" windowWidth="22980" windowHeight="9528"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="4" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="327">
   <si>
     <t>Plan</t>
   </si>
@@ -661,9 +661,6 @@
     <t>#15[increase]+#12[true]</t>
   </si>
   <si>
-    <t>#18[normal]+#19[False]+#20[False]+#21[False]+#21[normal]</t>
-  </si>
-  <si>
     <t>#22[horizontal]</t>
   </si>
   <si>
@@ -692,13 +689,429 @@
   </si>
   <si>
     <t>#9[normal]+#10[normal]+#13[normal]+#15[normal]</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>RHipAngles</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>RHipMoment</t>
+  </si>
+  <si>
+    <t>RKneeAngles</t>
+  </si>
+  <si>
+    <t>RKneeMoment</t>
+  </si>
+  <si>
+    <t>RAnkleAngles</t>
+  </si>
+  <si>
+    <t>Transverse plane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Excessive pelvic external rotation during the gait cycle </t>
+  </si>
+  <si>
+    <t>Excessive pelvic internal rotation during the gait cycle</t>
+  </si>
+  <si>
+    <t>Excessive hip external rotation during the gait cycle</t>
+  </si>
+  <si>
+    <t>Excessive hip internal rotation during the gait cycle</t>
+  </si>
+  <si>
+    <t>Foot</t>
+  </si>
+  <si>
+    <t>Normal foot progression angle</t>
+  </si>
+  <si>
+    <t>Outtoeing</t>
+  </si>
+  <si>
+    <t>Excessive external foot progression on average during stance</t>
+  </si>
+  <si>
+    <t>Intoeing</t>
+  </si>
+  <si>
+    <t>Excessive internal foot progression on average during stance</t>
+  </si>
+  <si>
+    <t>pelvic range of motion</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>hip abduction in swing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">continuous pelvic elevation </t>
+  </si>
+  <si>
+    <t>LFootProgressAngles</t>
+  </si>
+  <si>
+    <t>6,10</t>
+  </si>
+  <si>
+    <t>-9,-5</t>
+  </si>
+  <si>
+    <t>excessive,normal,insufficient</t>
+  </si>
+  <si>
+    <t>3,12</t>
+  </si>
+  <si>
+    <t>insufficient,normal,excessive</t>
+  </si>
+  <si>
+    <t>-4,4</t>
+  </si>
+  <si>
+    <t>-11,7</t>
+  </si>
+  <si>
+    <t>-12,1</t>
+  </si>
+  <si>
+    <t>#27[True]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">continuous pelvic depression </t>
+  </si>
+  <si>
+    <t>#25[normal]+#26[False]+#27[False]</t>
+  </si>
+  <si>
+    <t>#25[increase]</t>
+  </si>
+  <si>
+    <t>#26[True]</t>
+  </si>
+  <si>
+    <t>#28[excessive]</t>
+  </si>
+  <si>
+    <t>#29[True]</t>
+  </si>
+  <si>
+    <t>#30[True]</t>
+  </si>
+  <si>
+    <t>#28[normal]+#29[False]+#30[False]</t>
+  </si>
+  <si>
+    <t>#31[increase]</t>
+  </si>
+  <si>
+    <t>#32[excessive]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pelvic rotation during the gait cycle </t>
+  </si>
+  <si>
+    <t>#32[insufficient]</t>
+  </si>
+  <si>
+    <t>#31[normal]+#32[normal]</t>
+  </si>
+  <si>
+    <t>#33[excessive]</t>
+  </si>
+  <si>
+    <t>#33[insufficient]</t>
+  </si>
+  <si>
+    <t>#34[insufficient]</t>
+  </si>
+  <si>
+    <t>#33[normal]</t>
+  </si>
+  <si>
+    <t>#34[normal]</t>
+  </si>
+  <si>
+    <t>#34[excessive]</t>
+  </si>
+  <si>
+    <t>RFootProgressAngles</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>#35[normal]+#36[normal]+#39[False]+#40[False]</t>
+  </si>
+  <si>
+    <r>
+      <t>(#35[decrease]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>#36[decrease]</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>#37[delayed]|#38[decrease],2)</t>
+    </r>
+  </si>
+  <si>
+    <t>#39[True]+#40[True]</t>
+  </si>
+  <si>
+    <t>#41[normal]+#42[normal]+#45[normal]+#47[normal]</t>
+  </si>
+  <si>
+    <t>#41[increase]</t>
+  </si>
+  <si>
+    <t>#41[increase]+#42[early]</t>
+  </si>
+  <si>
+    <t>(#45[increase]|#42[early]|#46[excessive],2)</t>
+  </si>
+  <si>
+    <t>#41[increase]+(#45[increase]|#42[early]|#46[excessive],2)</t>
+  </si>
+  <si>
+    <t>#47[increase]+#43[true]</t>
+  </si>
+  <si>
+    <t>#47[increase]+#44[true]</t>
+  </si>
+  <si>
+    <t>#48[normal]+#49[normal]</t>
+  </si>
+  <si>
+    <t>#48[delayed]</t>
+  </si>
+  <si>
+    <t>#49[increase]</t>
+  </si>
+  <si>
+    <t>#48[delayed]+#49[increase]</t>
+  </si>
+  <si>
+    <t>#49[decrease]</t>
+  </si>
+  <si>
+    <t>#48[delayed]+#49[decrease]</t>
+  </si>
+  <si>
+    <t>#18[normal]+#19[False]+#20[False]+#21[False]+#22[normal]</t>
+  </si>
+  <si>
+    <t>#50[normal]+#51[False]+#52[False]+#53[False]+#54[normal]</t>
+  </si>
+  <si>
+    <t>#54[horizontal]</t>
+  </si>
+  <si>
+    <t>#54[descent]</t>
+  </si>
+  <si>
+    <t>#53[true]</t>
+  </si>
+  <si>
+    <t>(#52[True]|#51[True],1)</t>
+  </si>
+  <si>
+    <t>#55[true]</t>
+  </si>
+  <si>
+    <t>#50[excessive]</t>
+  </si>
+  <si>
+    <t>#56[true]+#50[excessive]</t>
+  </si>
+  <si>
+    <t>#57[normal]+#58[False]+#59[False]</t>
+  </si>
+  <si>
+    <t>#57[excessive]</t>
+  </si>
+  <si>
+    <t>#58[True]</t>
+  </si>
+  <si>
+    <t>#59[True]</t>
+  </si>
+  <si>
+    <t>#60[normal]</t>
+  </si>
+  <si>
+    <t>#60[excessive]</t>
+  </si>
+  <si>
+    <t>#60[insufficient]</t>
+  </si>
+  <si>
+    <t>#61[normal]</t>
+  </si>
+  <si>
+    <t>#61[excessive]</t>
+  </si>
+  <si>
+    <t>#61[insufficient]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -758,8 +1171,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -801,8 +1221,56 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -855,13 +1323,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="dashDot">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -943,53 +1438,248 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="13" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="14" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="15" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="14" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1294,10 +1984,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:N63"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="E31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1312,7 +2002,7 @@
     <col min="9" max="9" width="21.6640625" style="1" customWidth="1"/>
     <col min="10" max="10" width="16.88671875" style="1" customWidth="1"/>
     <col min="11" max="11" width="18.44140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="15.44140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="15.44140625" style="63" customWidth="1"/>
     <col min="13" max="13" width="46.6640625" style="1" customWidth="1"/>
     <col min="14" max="16384" width="8.88671875" style="1"/>
   </cols>
@@ -1359,7 +2049,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="38">
+      <c r="A2" s="34">
         <v>1</v>
       </c>
       <c r="B2" s="25" t="s">
@@ -1390,13 +2080,13 @@
         <v>5</v>
       </c>
       <c r="K2" s="25"/>
-      <c r="L2" s="25" t="s">
+      <c r="L2" s="34" t="s">
         <v>119</v>
       </c>
       <c r="M2" s="25"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="39">
+      <c r="A3" s="35">
         <v>2</v>
       </c>
       <c r="B3" s="26" t="s">
@@ -1427,13 +2117,13 @@
         <v>4</v>
       </c>
       <c r="K3" s="26"/>
-      <c r="L3" s="26" t="s">
+      <c r="L3" s="35" t="s">
         <v>120</v>
       </c>
       <c r="M3" s="26"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="38">
+      <c r="A4" s="47">
         <v>3</v>
       </c>
       <c r="B4" s="25" t="s">
@@ -1442,7 +2132,7 @@
       <c r="C4" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="43" t="s">
         <v>49</v>
       </c>
       <c r="E4" s="25" t="s">
@@ -1457,20 +2147,20 @@
       <c r="H4" s="25">
         <v>0</v>
       </c>
-      <c r="I4" s="31" t="s">
+      <c r="I4" s="43" t="s">
         <v>89</v>
       </c>
       <c r="J4" s="25" t="s">
         <v>6</v>
       </c>
       <c r="K4" s="25"/>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="34" t="s">
         <v>121</v>
       </c>
       <c r="M4" s="25"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="38">
+      <c r="A5" s="47">
         <v>4</v>
       </c>
       <c r="B5" s="25" t="s">
@@ -1479,7 +2169,7 @@
       <c r="C5" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="43" t="s">
         <v>75</v>
       </c>
       <c r="E5" s="25" t="s">
@@ -1494,20 +2184,20 @@
       <c r="H5" s="25">
         <v>0</v>
       </c>
-      <c r="I5" s="31" t="s">
+      <c r="I5" s="43" t="s">
         <v>89</v>
       </c>
       <c r="J5" s="25" t="s">
         <v>5</v>
       </c>
       <c r="K5" s="25"/>
-      <c r="L5" s="25" t="s">
+      <c r="L5" s="34" t="s">
         <v>122</v>
       </c>
       <c r="M5" s="25"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="40">
+      <c r="A6" s="48">
         <v>5</v>
       </c>
       <c r="B6" s="27" t="s">
@@ -1516,7 +2206,7 @@
       <c r="C6" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="D6" s="32" t="s">
+      <c r="D6" s="44" t="s">
         <v>111</v>
       </c>
       <c r="E6" s="27" t="s">
@@ -1531,7 +2221,7 @@
       <c r="H6" s="25">
         <v>0</v>
       </c>
-      <c r="I6" s="31" t="s">
+      <c r="I6" s="43" t="s">
         <v>89</v>
       </c>
       <c r="J6" s="25" t="s">
@@ -1540,13 +2230,13 @@
       <c r="K6" s="25">
         <v>0</v>
       </c>
-      <c r="L6" s="25" t="s">
+      <c r="L6" s="34" t="s">
         <v>123</v>
       </c>
       <c r="M6" s="25"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="40">
+      <c r="A7" s="48">
         <v>6</v>
       </c>
       <c r="B7" s="27" t="s">
@@ -1555,7 +2245,7 @@
       <c r="C7" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="44" t="s">
         <v>44</v>
       </c>
       <c r="E7" s="27" t="s">
@@ -1570,20 +2260,20 @@
       <c r="H7" s="25">
         <v>0</v>
       </c>
-      <c r="I7" s="31" t="s">
+      <c r="I7" s="43" t="s">
         <v>89</v>
       </c>
       <c r="J7" s="25" t="s">
         <v>6</v>
       </c>
       <c r="K7" s="25"/>
-      <c r="L7" s="25" t="s">
+      <c r="L7" s="34" t="s">
         <v>124</v>
       </c>
       <c r="M7" s="25"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="38">
+      <c r="A8" s="47">
         <v>7</v>
       </c>
       <c r="B8" s="25" t="s">
@@ -1614,11 +2304,11 @@
       <c r="K8" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="L8" s="25"/>
+      <c r="L8" s="34"/>
       <c r="M8" s="25"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="39">
+      <c r="A9" s="49">
         <v>8</v>
       </c>
       <c r="B9" s="26" t="s">
@@ -1649,11 +2339,11 @@
       <c r="K9" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="L9" s="26"/>
+      <c r="L9" s="35"/>
       <c r="M9" s="26"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="38">
+      <c r="A10" s="47">
         <v>9</v>
       </c>
       <c r="B10" s="25" t="s">
@@ -1686,22 +2376,22 @@
       <c r="K10" s="25">
         <v>0</v>
       </c>
-      <c r="L10" s="25" t="s">
+      <c r="L10" s="34" t="s">
         <v>125</v>
       </c>
       <c r="M10" s="25"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="38">
+      <c r="A11" s="47">
         <v>10</v>
       </c>
       <c r="B11" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="38" t="s">
+      <c r="C11" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="43" t="s">
         <v>187</v>
       </c>
       <c r="E11" s="25" t="s">
@@ -1716,27 +2406,27 @@
       <c r="H11" s="25">
         <v>0</v>
       </c>
-      <c r="I11" s="31" t="s">
+      <c r="I11" s="43" t="s">
         <v>89</v>
       </c>
       <c r="J11" s="25" t="s">
         <v>16</v>
       </c>
       <c r="K11" s="25"/>
-      <c r="L11" s="25" t="s">
+      <c r="L11" s="34" t="s">
         <v>126</v>
       </c>
       <c r="M11" s="25"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="48" t="s">
         <v>186</v>
       </c>
       <c r="B12" s="27" t="s">
         <v>103</v>
       </c>
       <c r="C12" s="27"/>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="44" t="s">
         <v>112</v>
       </c>
       <c r="E12" s="27" t="s">
@@ -1751,7 +2441,7 @@
       <c r="H12" s="25">
         <v>0</v>
       </c>
-      <c r="I12" s="31" t="s">
+      <c r="I12" s="43" t="s">
         <v>89</v>
       </c>
       <c r="J12" s="25" t="s">
@@ -1760,18 +2450,18 @@
       <c r="K12" s="25" t="s">
         <v>165</v>
       </c>
-      <c r="L12" s="25"/>
+      <c r="L12" s="34"/>
       <c r="M12" s="25"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="40" t="s">
+      <c r="A13" s="48" t="s">
         <v>166</v>
       </c>
       <c r="B13" s="27" t="s">
         <v>103</v>
       </c>
       <c r="C13" s="27"/>
-      <c r="D13" s="32" t="s">
+      <c r="D13" s="44" t="s">
         <v>17</v>
       </c>
       <c r="E13" s="27" t="s">
@@ -1786,7 +2476,7 @@
       <c r="H13" s="25">
         <v>0</v>
       </c>
-      <c r="I13" s="31" t="s">
+      <c r="I13" s="43" t="s">
         <v>89</v>
       </c>
       <c r="J13" s="25" t="s">
@@ -1795,11 +2485,11 @@
       <c r="K13" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="L13" s="25"/>
+      <c r="L13" s="34"/>
       <c r="M13" s="25"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="47" t="s">
         <v>167</v>
       </c>
       <c r="B14" s="25" t="s">
@@ -1808,7 +2498,7 @@
       <c r="C14" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="42" t="s">
         <v>47</v>
       </c>
       <c r="E14" s="25" t="s">
@@ -1823,20 +2513,20 @@
       <c r="H14" s="25">
         <v>0</v>
       </c>
-      <c r="I14" s="28" t="s">
+      <c r="I14" s="42" t="s">
         <v>137</v>
       </c>
       <c r="J14" s="25" t="s">
         <v>6</v>
       </c>
       <c r="K14" s="25"/>
-      <c r="L14" s="25" t="s">
+      <c r="L14" s="34" t="s">
         <v>127</v>
       </c>
       <c r="M14" s="25"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="40" t="s">
+      <c r="A15" s="48" t="s">
         <v>168</v>
       </c>
       <c r="B15" s="27" t="s">
@@ -1845,7 +2535,7 @@
       <c r="C15" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="D15" s="37" t="s">
+      <c r="D15" s="45" t="s">
         <v>107</v>
       </c>
       <c r="E15" s="27" t="s">
@@ -1860,20 +2550,20 @@
       <c r="H15" s="25">
         <v>0</v>
       </c>
-      <c r="I15" s="28" t="s">
+      <c r="I15" s="42" t="s">
         <v>137</v>
       </c>
       <c r="J15" s="25" t="s">
         <v>6</v>
       </c>
       <c r="K15" s="25"/>
-      <c r="L15" s="25" t="s">
+      <c r="L15" s="34" t="s">
         <v>128</v>
       </c>
       <c r="M15" s="25"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="47" t="s">
         <v>169</v>
       </c>
       <c r="B16" s="25" t="s">
@@ -1882,7 +2572,7 @@
       <c r="C16" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="D16" s="28" t="s">
+      <c r="D16" s="42" t="s">
         <v>108</v>
       </c>
       <c r="E16" s="25" t="s">
@@ -1897,20 +2587,20 @@
       <c r="H16" s="25">
         <v>0</v>
       </c>
-      <c r="I16" s="28" t="s">
+      <c r="I16" s="42" t="s">
         <v>136</v>
       </c>
       <c r="J16" s="25" t="s">
         <v>7</v>
       </c>
       <c r="K16" s="25"/>
-      <c r="L16" s="25" t="s">
+      <c r="L16" s="34" t="s">
         <v>129</v>
       </c>
       <c r="M16" s="25"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="38" t="s">
+      <c r="A17" s="47" t="s">
         <v>170</v>
       </c>
       <c r="B17" s="25" t="s">
@@ -1919,7 +2609,7 @@
       <c r="C17" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="D17" s="29" t="s">
+      <c r="D17" s="41" t="s">
         <v>48</v>
       </c>
       <c r="E17" s="25" t="s">
@@ -1934,20 +2624,20 @@
       <c r="H17" s="25">
         <v>0</v>
       </c>
-      <c r="I17" s="29" t="s">
+      <c r="I17" s="41" t="s">
         <v>90</v>
       </c>
       <c r="J17" s="25" t="s">
         <v>15</v>
       </c>
       <c r="K17" s="25"/>
-      <c r="L17" s="25" t="s">
+      <c r="L17" s="34" t="s">
         <v>131</v>
       </c>
       <c r="M17" s="25"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="39" t="s">
+      <c r="A18" s="49" t="s">
         <v>171</v>
       </c>
       <c r="B18" s="26" t="s">
@@ -1956,7 +2646,7 @@
       <c r="C18" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="D18" s="30" t="s">
+      <c r="D18" s="46" t="s">
         <v>48</v>
       </c>
       <c r="E18" s="26" t="s">
@@ -1971,20 +2661,20 @@
       <c r="H18" s="26">
         <v>0</v>
       </c>
-      <c r="I18" s="30" t="s">
+      <c r="I18" s="46" t="s">
         <v>90</v>
       </c>
       <c r="J18" s="26" t="s">
         <v>7</v>
       </c>
       <c r="K18" s="26"/>
-      <c r="L18" s="26" t="s">
+      <c r="L18" s="35" t="s">
         <v>130</v>
       </c>
       <c r="M18" s="26"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="38" t="s">
+      <c r="A19" s="47" t="s">
         <v>172</v>
       </c>
       <c r="B19" s="25" t="s">
@@ -2017,20 +2707,20 @@
       <c r="K19" s="25">
         <v>100</v>
       </c>
-      <c r="L19" s="25" t="s">
+      <c r="L19" s="34" t="s">
         <v>135</v>
       </c>
       <c r="M19" s="25"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="38" t="s">
+      <c r="A20" s="47" t="s">
         <v>173</v>
       </c>
       <c r="B20" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C20" s="25"/>
-      <c r="D20" s="31" t="s">
+      <c r="D20" s="43" t="s">
         <v>66</v>
       </c>
       <c r="E20" s="25" t="s">
@@ -2045,7 +2735,7 @@
       <c r="H20" s="25">
         <v>0</v>
       </c>
-      <c r="I20" s="31" t="s">
+      <c r="I20" s="43" t="s">
         <v>89</v>
       </c>
       <c r="J20" s="25" t="s">
@@ -2054,18 +2744,18 @@
       <c r="K20" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="L20" s="25"/>
+      <c r="L20" s="34"/>
       <c r="M20" s="25"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="38" t="s">
+      <c r="A21" s="47" t="s">
         <v>174</v>
       </c>
       <c r="B21" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C21" s="25"/>
-      <c r="D21" s="31" t="s">
+      <c r="D21" s="43" t="s">
         <v>132</v>
       </c>
       <c r="E21" s="25" t="s">
@@ -2080,7 +2770,7 @@
       <c r="H21" s="25">
         <v>0</v>
       </c>
-      <c r="I21" s="31" t="s">
+      <c r="I21" s="43" t="s">
         <v>89</v>
       </c>
       <c r="J21" s="25" t="s">
@@ -2089,18 +2779,18 @@
       <c r="K21" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="L21" s="25"/>
+      <c r="L21" s="34"/>
       <c r="M21" s="25"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="38" t="s">
+      <c r="A22" s="47" t="s">
         <v>144</v>
       </c>
       <c r="B22" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C22" s="25"/>
-      <c r="D22" s="31" t="s">
+      <c r="D22" s="43" t="s">
         <v>74</v>
       </c>
       <c r="E22" s="25" t="s">
@@ -2115,7 +2805,7 @@
       <c r="H22" s="25">
         <v>0</v>
       </c>
-      <c r="I22" s="31" t="s">
+      <c r="I22" s="43" t="s">
         <v>89</v>
       </c>
       <c r="J22" s="25" t="s">
@@ -2124,11 +2814,11 @@
       <c r="K22" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="L22" s="25"/>
+      <c r="L22" s="34"/>
       <c r="M22" s="25"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="38" t="s">
+      <c r="A23" s="47" t="s">
         <v>145</v>
       </c>
       <c r="B23" s="25" t="s">
@@ -2137,7 +2827,7 @@
       <c r="C23" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="D23" s="28" t="s">
+      <c r="D23" s="42" t="s">
         <v>109</v>
       </c>
       <c r="E23" s="25" t="s">
@@ -2152,20 +2842,20 @@
       <c r="H23" s="25">
         <v>0</v>
       </c>
-      <c r="I23" s="28" t="s">
+      <c r="I23" s="42" t="s">
         <v>143</v>
       </c>
       <c r="J23" s="25" t="s">
         <v>133</v>
       </c>
       <c r="K23" s="25"/>
-      <c r="L23" s="25" t="s">
+      <c r="L23" s="34" t="s">
         <v>117</v>
       </c>
       <c r="M23" s="25"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="38" t="s">
+      <c r="A24" s="47" t="s">
         <v>146</v>
       </c>
       <c r="B24" s="25" t="s">
@@ -2174,7 +2864,7 @@
       <c r="C24" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="D24" s="29" t="s">
+      <c r="D24" s="41" t="s">
         <v>87</v>
       </c>
       <c r="E24" s="25" t="s">
@@ -2189,7 +2879,7 @@
       <c r="H24" s="25">
         <v>0</v>
       </c>
-      <c r="I24" s="29" t="s">
+      <c r="I24" s="41" t="s">
         <v>90</v>
       </c>
       <c r="J24" s="25" t="s">
@@ -2198,41 +2888,1365 @@
       <c r="K24" s="25" t="s">
         <v>140</v>
       </c>
-      <c r="L24" s="25"/>
+      <c r="L24" s="34"/>
       <c r="M24" s="25"/>
     </row>
-    <row r="25" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="38" t="s">
-        <v>200</v>
-      </c>
-      <c r="B25" s="38" t="s">
+    <row r="25" spans="1:13" s="40" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="78" t="s">
+        <v>199</v>
+      </c>
+      <c r="B25" s="79" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="41" t="s">
-        <v>199</v>
-      </c>
-      <c r="E25" s="38" t="s">
-        <v>92</v>
-      </c>
-      <c r="F25" s="38" t="s">
+      <c r="C25" s="80"/>
+      <c r="D25" s="81" t="s">
+        <v>198</v>
+      </c>
+      <c r="E25" s="79" t="s">
+        <v>92</v>
+      </c>
+      <c r="F25" s="79" t="s">
         <v>99</v>
       </c>
-      <c r="G25" s="38">
-        <v>0</v>
-      </c>
-      <c r="H25" s="38">
-        <v>0</v>
-      </c>
-      <c r="I25" s="41" t="s">
+      <c r="G25" s="79">
+        <v>0</v>
+      </c>
+      <c r="H25" s="79">
+        <v>0</v>
+      </c>
+      <c r="I25" s="81" t="s">
         <v>90</v>
       </c>
-      <c r="J25" s="38" t="s">
+      <c r="J25" s="79" t="s">
         <v>69</v>
       </c>
-      <c r="K25" s="38" t="s">
+      <c r="K25" s="79" t="s">
         <v>141</v>
       </c>
-    </row>
+      <c r="L25" s="82"/>
+      <c r="M25" s="80"/>
+    </row>
+    <row r="26" spans="1:13" s="58" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="56" t="s">
+        <v>203</v>
+      </c>
+      <c r="B26" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" s="57" t="s">
+        <v>115</v>
+      </c>
+      <c r="D26" s="59" t="s">
+        <v>242</v>
+      </c>
+      <c r="E26" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="F26" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="G26" s="57" t="s">
+        <v>134</v>
+      </c>
+      <c r="H26" s="57" t="s">
+        <v>243</v>
+      </c>
+      <c r="I26" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="J26" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="K26" s="57"/>
+      <c r="L26" s="61" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" s="58" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="56" t="s">
+        <v>204</v>
+      </c>
+      <c r="B27" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="59" t="s">
+        <v>246</v>
+      </c>
+      <c r="E27" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="F27" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="G27" s="57" t="s">
+        <v>134</v>
+      </c>
+      <c r="H27" s="57" t="s">
+        <v>243</v>
+      </c>
+      <c r="I27" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="J27" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="K27" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="L27" s="62"/>
+    </row>
+    <row r="28" spans="1:13" s="58" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="56" t="s">
+        <v>205</v>
+      </c>
+      <c r="B28" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="59" t="s">
+        <v>257</v>
+      </c>
+      <c r="E28" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="F28" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="G28" s="57" t="s">
+        <v>134</v>
+      </c>
+      <c r="H28" s="57" t="s">
+        <v>243</v>
+      </c>
+      <c r="I28" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="J28" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="K28" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="L28" s="62"/>
+    </row>
+    <row r="29" spans="1:13" s="58" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="56" t="s">
+        <v>206</v>
+      </c>
+      <c r="B29" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="D29" s="59" t="s">
+        <v>245</v>
+      </c>
+      <c r="E29" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="F29" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="G29" s="57" t="s">
+        <v>134</v>
+      </c>
+      <c r="H29" s="57" t="s">
+        <v>243</v>
+      </c>
+      <c r="I29" s="41" t="s">
+        <v>90</v>
+      </c>
+      <c r="J29" s="57" t="s">
+        <v>6</v>
+      </c>
+      <c r="K29" s="57"/>
+      <c r="L29" s="62" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" s="58" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="56" t="s">
+        <v>207</v>
+      </c>
+      <c r="B30" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="59" t="s">
+        <v>80</v>
+      </c>
+      <c r="E30" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="F30" s="57" t="s">
+        <v>97</v>
+      </c>
+      <c r="G30" s="57" t="s">
+        <v>134</v>
+      </c>
+      <c r="H30" s="57" t="s">
+        <v>243</v>
+      </c>
+      <c r="I30" s="57" t="s">
+        <v>46</v>
+      </c>
+      <c r="J30" s="57" t="s">
+        <v>69</v>
+      </c>
+      <c r="K30" s="57" t="s">
+        <v>142</v>
+      </c>
+      <c r="L30" s="62"/>
+    </row>
+    <row r="31" spans="1:13" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="78" t="s">
+        <v>208</v>
+      </c>
+      <c r="B31" s="79" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="80"/>
+      <c r="D31" s="83" t="s">
+        <v>81</v>
+      </c>
+      <c r="E31" s="79" t="s">
+        <v>92</v>
+      </c>
+      <c r="F31" s="79" t="s">
+        <v>97</v>
+      </c>
+      <c r="G31" s="79" t="s">
+        <v>134</v>
+      </c>
+      <c r="H31" s="57" t="s">
+        <v>243</v>
+      </c>
+      <c r="I31" s="79" t="s">
+        <v>46</v>
+      </c>
+      <c r="J31" s="79" t="s">
+        <v>69</v>
+      </c>
+      <c r="K31" s="79" t="s">
+        <v>139</v>
+      </c>
+      <c r="L31" s="82"/>
+      <c r="M31" s="80"/>
+    </row>
+    <row r="32" spans="1:13" s="58" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="56" t="s">
+        <v>209</v>
+      </c>
+      <c r="B32" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="57" t="s">
+        <v>115</v>
+      </c>
+      <c r="D32" s="59" t="s">
+        <v>76</v>
+      </c>
+      <c r="E32" s="57" t="s">
+        <v>92</v>
+      </c>
+      <c r="F32" s="57" t="s">
+        <v>88</v>
+      </c>
+      <c r="G32" s="57" t="s">
+        <v>134</v>
+      </c>
+      <c r="H32" s="57" t="s">
+        <v>244</v>
+      </c>
+      <c r="I32" s="57" t="s">
+        <v>46</v>
+      </c>
+      <c r="J32" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="K32" s="57"/>
+      <c r="L32" s="62" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" s="58" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="56" t="s">
+        <v>210</v>
+      </c>
+      <c r="B33" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" s="34" t="s">
+        <v>252</v>
+      </c>
+      <c r="D33" s="59" t="s">
+        <v>267</v>
+      </c>
+      <c r="E33" s="57" t="s">
+        <v>92</v>
+      </c>
+      <c r="F33" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="G33" s="57" t="s">
+        <v>134</v>
+      </c>
+      <c r="H33" s="57" t="s">
+        <v>244</v>
+      </c>
+      <c r="I33" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="J33" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="K33" s="57"/>
+      <c r="L33" s="62" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" s="58" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="56" t="s">
+        <v>211</v>
+      </c>
+      <c r="B34" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" s="34" t="s">
+        <v>252</v>
+      </c>
+      <c r="D34" s="59" t="s">
+        <v>234</v>
+      </c>
+      <c r="E34" s="57" t="s">
+        <v>92</v>
+      </c>
+      <c r="F34" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="G34" s="57" t="s">
+        <v>134</v>
+      </c>
+      <c r="H34" s="57" t="s">
+        <v>244</v>
+      </c>
+      <c r="I34" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="J34" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="K34" s="57"/>
+      <c r="L34" s="62" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" s="80" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="78" t="s">
+        <v>212</v>
+      </c>
+      <c r="B35" s="79" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="79" t="s">
+        <v>252</v>
+      </c>
+      <c r="D35" s="83" t="s">
+        <v>239</v>
+      </c>
+      <c r="E35" s="79" t="s">
+        <v>92</v>
+      </c>
+      <c r="F35" s="79" t="s">
+        <v>247</v>
+      </c>
+      <c r="G35" s="79" t="s">
+        <v>134</v>
+      </c>
+      <c r="H35" s="79" t="s">
+        <v>244</v>
+      </c>
+      <c r="I35" s="87" t="s">
+        <v>89</v>
+      </c>
+      <c r="J35" s="79" t="s">
+        <v>4</v>
+      </c>
+      <c r="K35" s="79"/>
+      <c r="L35" s="82" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="50" t="s">
+        <v>213</v>
+      </c>
+      <c r="B36" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="D36" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="E36" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="F36" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="G36" s="34">
+        <v>0</v>
+      </c>
+      <c r="H36" s="34">
+        <v>0</v>
+      </c>
+      <c r="I36" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="J36" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="K36" s="34"/>
+      <c r="L36" s="34" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37" s="50" t="s">
+        <v>214</v>
+      </c>
+      <c r="B37" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="D37" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="E37" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="F37" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="G37" s="34">
+        <v>0</v>
+      </c>
+      <c r="H37" s="34">
+        <v>0</v>
+      </c>
+      <c r="I37" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="J37" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="K37" s="34"/>
+      <c r="L37" s="34" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38" s="50" t="s">
+        <v>215</v>
+      </c>
+      <c r="B38" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="C38" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="D38" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="E38" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="F38" s="36" t="s">
+        <v>227</v>
+      </c>
+      <c r="G38" s="34">
+        <v>0</v>
+      </c>
+      <c r="H38" s="34">
+        <v>0</v>
+      </c>
+      <c r="I38" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="J38" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="K38" s="34">
+        <v>0</v>
+      </c>
+      <c r="L38" s="34" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A39" s="50" t="s">
+        <v>216</v>
+      </c>
+      <c r="B39" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="C39" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="D39" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="E39" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="F39" s="36" t="s">
+        <v>227</v>
+      </c>
+      <c r="G39" s="34">
+        <v>0</v>
+      </c>
+      <c r="H39" s="34">
+        <v>0</v>
+      </c>
+      <c r="I39" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="J39" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="K39" s="34"/>
+      <c r="L39" s="34" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A40" s="50" t="s">
+        <v>217</v>
+      </c>
+      <c r="B40" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40" s="34"/>
+      <c r="D40" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="E40" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="F40" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="G40" s="34">
+        <v>0</v>
+      </c>
+      <c r="H40" s="34">
+        <v>0</v>
+      </c>
+      <c r="I40" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="J40" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="K40" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="L40" s="34"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41" s="50" t="s">
+        <v>218</v>
+      </c>
+      <c r="B41" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" s="35"/>
+      <c r="D41" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="E41" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="F41" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="G41" s="35">
+        <v>0</v>
+      </c>
+      <c r="H41" s="35">
+        <v>0</v>
+      </c>
+      <c r="I41" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="J41" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="K41" s="35" t="s">
+        <v>139</v>
+      </c>
+      <c r="L41" s="35"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A42" s="50" t="s">
+        <v>219</v>
+      </c>
+      <c r="B42" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="D42" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="E42" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="F42" s="34" t="s">
+        <v>228</v>
+      </c>
+      <c r="G42" s="34">
+        <v>0</v>
+      </c>
+      <c r="H42" s="34">
+        <v>0</v>
+      </c>
+      <c r="I42" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="J42" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="K42" s="34">
+        <v>0</v>
+      </c>
+      <c r="L42" s="34" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A43" s="50" t="s">
+        <v>220</v>
+      </c>
+      <c r="B43" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="D43" s="30" t="s">
+        <v>187</v>
+      </c>
+      <c r="E43" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="F43" s="34" t="s">
+        <v>228</v>
+      </c>
+      <c r="G43" s="34">
+        <v>0</v>
+      </c>
+      <c r="H43" s="34">
+        <v>0</v>
+      </c>
+      <c r="I43" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="J43" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="K43" s="34"/>
+      <c r="L43" s="34" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A44" s="50" t="s">
+        <v>221</v>
+      </c>
+      <c r="B44" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="C44" s="36"/>
+      <c r="D44" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="E44" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="F44" s="36" t="s">
+        <v>229</v>
+      </c>
+      <c r="G44" s="34">
+        <v>0</v>
+      </c>
+      <c r="H44" s="34">
+        <v>0</v>
+      </c>
+      <c r="I44" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="J44" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="K44" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="L44" s="34"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A45" s="50" t="s">
+        <v>222</v>
+      </c>
+      <c r="B45" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="C45" s="36"/>
+      <c r="D45" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="E45" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="F45" s="36" t="s">
+        <v>229</v>
+      </c>
+      <c r="G45" s="34">
+        <v>0</v>
+      </c>
+      <c r="H45" s="34">
+        <v>0</v>
+      </c>
+      <c r="I45" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="J45" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="K45" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="L45" s="34"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A46" s="50" t="s">
+        <v>223</v>
+      </c>
+      <c r="B46" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="D46" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="E46" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="F46" s="34" t="s">
+        <v>228</v>
+      </c>
+      <c r="G46" s="34">
+        <v>0</v>
+      </c>
+      <c r="H46" s="34">
+        <v>0</v>
+      </c>
+      <c r="I46" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="J46" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="K46" s="34"/>
+      <c r="L46" s="34" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A47" s="50" t="s">
+        <v>224</v>
+      </c>
+      <c r="B47" s="36" t="s">
+        <v>103</v>
+      </c>
+      <c r="C47" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="D47" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="E47" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="F47" s="36" t="s">
+        <v>229</v>
+      </c>
+      <c r="G47" s="34">
+        <v>0</v>
+      </c>
+      <c r="H47" s="34">
+        <v>0</v>
+      </c>
+      <c r="I47" s="28" t="s">
+        <v>137</v>
+      </c>
+      <c r="J47" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="K47" s="34"/>
+      <c r="L47" s="34" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A48" s="50" t="s">
+        <v>277</v>
+      </c>
+      <c r="B48" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="D48" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="E48" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="F48" s="34" t="s">
+        <v>228</v>
+      </c>
+      <c r="G48" s="34">
+        <v>0</v>
+      </c>
+      <c r="H48" s="34">
+        <v>0</v>
+      </c>
+      <c r="I48" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="J48" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="K48" s="34"/>
+      <c r="L48" s="34" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A49" s="50" t="s">
+        <v>278</v>
+      </c>
+      <c r="B49" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C49" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="D49" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="E49" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="F49" s="34" t="s">
+        <v>228</v>
+      </c>
+      <c r="G49" s="34">
+        <v>0</v>
+      </c>
+      <c r="H49" s="34">
+        <v>0</v>
+      </c>
+      <c r="I49" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="J49" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="K49" s="34"/>
+      <c r="L49" s="34" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A50" s="50" t="s">
+        <v>279</v>
+      </c>
+      <c r="B50" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="C50" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="D50" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="E50" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="F50" s="34" t="s">
+        <v>228</v>
+      </c>
+      <c r="G50" s="35">
+        <v>0</v>
+      </c>
+      <c r="H50" s="35">
+        <v>0</v>
+      </c>
+      <c r="I50" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="J50" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="K50" s="35"/>
+      <c r="L50" s="35" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A51" s="50" t="s">
+        <v>280</v>
+      </c>
+      <c r="B51" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C51" s="34" t="s">
+        <v>116</v>
+      </c>
+      <c r="D51" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="E51" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="F51" s="34" t="s">
+        <v>230</v>
+      </c>
+      <c r="G51" s="34">
+        <v>0</v>
+      </c>
+      <c r="H51" s="34">
+        <v>0</v>
+      </c>
+      <c r="I51" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="J51" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="K51" s="34">
+        <v>100</v>
+      </c>
+      <c r="L51" s="34" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A52" s="50" t="s">
+        <v>281</v>
+      </c>
+      <c r="B52" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C52" s="34"/>
+      <c r="D52" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="E52" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="F52" s="34" t="s">
+        <v>230</v>
+      </c>
+      <c r="G52" s="34">
+        <v>0</v>
+      </c>
+      <c r="H52" s="34">
+        <v>0</v>
+      </c>
+      <c r="I52" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="J52" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="K52" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="L52" s="34"/>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A53" s="50" t="s">
+        <v>282</v>
+      </c>
+      <c r="B53" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C53" s="34"/>
+      <c r="D53" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="E53" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="F53" s="34" t="s">
+        <v>230</v>
+      </c>
+      <c r="G53" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="H53" s="34">
+        <v>0</v>
+      </c>
+      <c r="I53" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="J53" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="K53" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="L53" s="34"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A54" s="50" t="s">
+        <v>283</v>
+      </c>
+      <c r="B54" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C54" s="34"/>
+      <c r="D54" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="E54" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="F54" s="34" t="s">
+        <v>230</v>
+      </c>
+      <c r="G54" s="34">
+        <v>0</v>
+      </c>
+      <c r="H54" s="34">
+        <v>0</v>
+      </c>
+      <c r="I54" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="J54" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="K54" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="L54" s="34"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A55" s="50" t="s">
+        <v>284</v>
+      </c>
+      <c r="B55" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C55" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="D55" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="E55" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="F55" s="34" t="s">
+        <v>230</v>
+      </c>
+      <c r="G55" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="H55" s="34">
+        <v>0</v>
+      </c>
+      <c r="I55" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="J55" s="34" t="s">
+        <v>133</v>
+      </c>
+      <c r="K55" s="34"/>
+      <c r="L55" s="34" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A56" s="50" t="s">
+        <v>285</v>
+      </c>
+      <c r="B56" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C56" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="D56" s="37" t="s">
+        <v>87</v>
+      </c>
+      <c r="E56" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="F56" s="34" t="s">
+        <v>230</v>
+      </c>
+      <c r="G56" s="34">
+        <v>0</v>
+      </c>
+      <c r="H56" s="34">
+        <v>0</v>
+      </c>
+      <c r="I56" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="J56" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="K56" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="L56" s="34"/>
+    </row>
+    <row r="57" spans="1:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="50" t="s">
+        <v>286</v>
+      </c>
+      <c r="B57" s="79" t="s">
+        <v>13</v>
+      </c>
+      <c r="C57" s="80"/>
+      <c r="D57" s="88" t="s">
+        <v>198</v>
+      </c>
+      <c r="E57" s="79" t="s">
+        <v>226</v>
+      </c>
+      <c r="F57" s="79" t="s">
+        <v>230</v>
+      </c>
+      <c r="G57" s="79">
+        <v>0</v>
+      </c>
+      <c r="H57" s="79">
+        <v>0</v>
+      </c>
+      <c r="I57" s="88" t="s">
+        <v>90</v>
+      </c>
+      <c r="J57" s="79" t="s">
+        <v>69</v>
+      </c>
+      <c r="K57" s="79" t="s">
+        <v>141</v>
+      </c>
+      <c r="L57" s="82"/>
+    </row>
+    <row r="58" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="50" t="s">
+        <v>287</v>
+      </c>
+      <c r="B58" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C58" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="D58" s="90" t="s">
+        <v>245</v>
+      </c>
+      <c r="E58" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="F58" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="G58" s="57" t="s">
+        <v>134</v>
+      </c>
+      <c r="H58" s="57" t="s">
+        <v>243</v>
+      </c>
+      <c r="I58" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="J58" s="57" t="s">
+        <v>6</v>
+      </c>
+      <c r="K58" s="57"/>
+      <c r="L58" s="62" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A59" s="50" t="s">
+        <v>288</v>
+      </c>
+      <c r="B59" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C59" s="58"/>
+      <c r="D59" s="59" t="s">
+        <v>80</v>
+      </c>
+      <c r="E59" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="F59" s="57" t="s">
+        <v>225</v>
+      </c>
+      <c r="G59" s="57" t="s">
+        <v>134</v>
+      </c>
+      <c r="H59" s="57" t="s">
+        <v>243</v>
+      </c>
+      <c r="I59" s="57" t="s">
+        <v>46</v>
+      </c>
+      <c r="J59" s="57" t="s">
+        <v>69</v>
+      </c>
+      <c r="K59" s="57" t="s">
+        <v>142</v>
+      </c>
+      <c r="L59" s="62"/>
+    </row>
+    <row r="60" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="50" t="s">
+        <v>289</v>
+      </c>
+      <c r="B60" s="79" t="s">
+        <v>13</v>
+      </c>
+      <c r="C60" s="80"/>
+      <c r="D60" s="83" t="s">
+        <v>81</v>
+      </c>
+      <c r="E60" s="79" t="s">
+        <v>226</v>
+      </c>
+      <c r="F60" s="57" t="s">
+        <v>225</v>
+      </c>
+      <c r="G60" s="79" t="s">
+        <v>134</v>
+      </c>
+      <c r="H60" s="57" t="s">
+        <v>243</v>
+      </c>
+      <c r="I60" s="79" t="s">
+        <v>46</v>
+      </c>
+      <c r="J60" s="79" t="s">
+        <v>69</v>
+      </c>
+      <c r="K60" s="79" t="s">
+        <v>139</v>
+      </c>
+      <c r="L60" s="82"/>
+    </row>
+    <row r="61" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="50" t="s">
+        <v>290</v>
+      </c>
+      <c r="B61" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C61" s="34" t="s">
+        <v>252</v>
+      </c>
+      <c r="D61" s="59" t="s">
+        <v>234</v>
+      </c>
+      <c r="E61" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="F61" s="57" t="s">
+        <v>225</v>
+      </c>
+      <c r="G61" s="57" t="s">
+        <v>134</v>
+      </c>
+      <c r="H61" s="57" t="s">
+        <v>244</v>
+      </c>
+      <c r="I61" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="J61" s="35" t="s">
+        <v>4</v>
+      </c>
+      <c r="K61" s="57"/>
+      <c r="L61" s="62" t="s">
+        <v>254</v>
+      </c>
+      <c r="M61" s="62" t="s">
+        <v>254</v>
+      </c>
+      <c r="N61" s="62" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="50" t="s">
+        <v>291</v>
+      </c>
+      <c r="B62" s="79" t="s">
+        <v>13</v>
+      </c>
+      <c r="C62" s="79" t="s">
+        <v>252</v>
+      </c>
+      <c r="D62" s="83" t="s">
+        <v>239</v>
+      </c>
+      <c r="E62" s="79" t="s">
+        <v>226</v>
+      </c>
+      <c r="F62" s="79" t="s">
+        <v>276</v>
+      </c>
+      <c r="G62" s="79" t="s">
+        <v>134</v>
+      </c>
+      <c r="H62" s="79" t="s">
+        <v>244</v>
+      </c>
+      <c r="I62" s="89" t="s">
+        <v>89</v>
+      </c>
+      <c r="J62" s="79" t="s">
+        <v>4</v>
+      </c>
+      <c r="K62" s="79"/>
+      <c r="L62" s="82" t="s">
+        <v>255</v>
+      </c>
+      <c r="M62" s="82" t="s">
+        <v>255</v>
+      </c>
+      <c r="N62" s="82" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2241,10 +4255,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView topLeftCell="A64" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2285,7 +4299,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="101" t="s">
         <v>84</v>
       </c>
       <c r="B2" s="22" t="s">
@@ -2294,19 +4308,16 @@
       <c r="C2" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="32" t="s">
         <v>70</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="32" t="s">
         <v>156</v>
       </c>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
     </row>
     <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="22" t="s">
-        <v>84</v>
-      </c>
       <c r="B3" s="22" t="s">
         <v>10</v>
       </c>
@@ -2321,9 +4332,6 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="22" t="s">
-        <v>84</v>
-      </c>
       <c r="B4" s="22" t="s">
         <v>10</v>
       </c>
@@ -2338,9 +4346,6 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="22" t="s">
-        <v>84</v>
-      </c>
       <c r="B5" s="22" t="s">
         <v>10</v>
       </c>
@@ -2355,9 +4360,6 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="22" t="s">
-        <v>84</v>
-      </c>
       <c r="B6" s="22" t="s">
         <v>10</v>
       </c>
@@ -2372,9 +4374,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="23" t="s">
-        <v>84</v>
-      </c>
+      <c r="A7" s="23"/>
       <c r="B7" s="23" t="s">
         <v>10</v>
       </c>
@@ -2392,34 +4392,28 @@
       <c r="H7" s="23"/>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="22" t="s">
-        <v>84</v>
-      </c>
       <c r="B8" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="C8" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="E8" s="36" t="s">
+      <c r="C8" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="E8" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="F8" s="36" t="s">
+      <c r="F8" s="32" t="s">
         <v>185</v>
       </c>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42" t="s">
-        <v>202</v>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="22" t="s">
-        <v>84</v>
-      </c>
       <c r="B9" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="54" t="s">
         <v>92</v>
       </c>
       <c r="E9" s="22" t="s">
@@ -2433,106 +4427,94 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="B10" s="22" t="s">
+      <c r="A10" s="103"/>
+      <c r="B10" s="103" t="s">
         <v>85</v>
       </c>
-      <c r="C10" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="E10" s="22" t="s">
+      <c r="C10" s="106" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" s="103"/>
+      <c r="E10" s="103" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="22" t="s">
+      <c r="F10" s="103" t="s">
         <v>163</v>
       </c>
-      <c r="G10" s="22" t="s">
+      <c r="G10" s="103" t="s">
         <v>31</v>
       </c>
+      <c r="H10" s="103"/>
     </row>
     <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="22" t="s">
-        <v>84</v>
-      </c>
       <c r="B11" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="D11" s="34" t="s">
+      <c r="C11" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" s="51" t="s">
         <v>153</v>
       </c>
-      <c r="E11" s="36" t="s">
+      <c r="E11" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="F11" s="36" t="s">
-        <v>203</v>
-      </c>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42" t="s">
+      <c r="F11" s="32" t="s">
         <v>202</v>
       </c>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="22" t="s">
-        <v>84</v>
-      </c>
       <c r="B12" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="D12" s="34" t="s">
+      <c r="C12" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" s="51" t="s">
         <v>153</v>
       </c>
-      <c r="E12" s="34" t="s">
+      <c r="E12" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="34" t="s">
+      <c r="F12" s="51" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="22" t="s">
-        <v>84</v>
-      </c>
       <c r="B13" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="D13" s="34" t="s">
+      <c r="C13" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" s="51" t="s">
         <v>153</v>
       </c>
-      <c r="E13" s="34" t="s">
+      <c r="E13" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="34" t="s">
+      <c r="F13" s="51" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="22" t="s">
-        <v>84</v>
-      </c>
       <c r="B14" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="D14" s="34" t="s">
+      <c r="C14" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" s="51" t="s">
         <v>153</v>
       </c>
-      <c r="E14" s="34" t="s">
+      <c r="E14" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="34" t="s">
+      <c r="F14" s="51" t="s">
         <v>189</v>
       </c>
       <c r="G14" s="22" t="s">
@@ -2540,22 +4522,19 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="22" t="s">
-        <v>84</v>
-      </c>
       <c r="B15" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="D15" s="34" t="s">
+      <c r="C15" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" s="51" t="s">
         <v>153</v>
       </c>
-      <c r="E15" s="34" t="s">
+      <c r="E15" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="34" t="s">
+      <c r="F15" s="51" t="s">
         <v>190</v>
       </c>
       <c r="G15" s="22" t="s">
@@ -2563,22 +4542,19 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="22" t="s">
-        <v>84</v>
-      </c>
       <c r="B16" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="D16" s="34" t="s">
+      <c r="C16" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="51" t="s">
         <v>153</v>
       </c>
-      <c r="E16" s="34" t="s">
+      <c r="E16" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="34" t="s">
+      <c r="F16" s="51" t="s">
         <v>191</v>
       </c>
       <c r="G16" s="22" t="s">
@@ -2586,365 +4562,1260 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="107" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="D17" s="34" t="s">
+      <c r="C17" s="108" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="109" t="s">
         <v>153</v>
       </c>
-      <c r="E17" s="34" t="s">
+      <c r="E17" s="109" t="s">
         <v>40</v>
       </c>
-      <c r="F17" s="34" t="s">
+      <c r="F17" s="109" t="s">
         <v>192</v>
       </c>
-      <c r="G17" s="22" t="s">
+      <c r="G17" s="107" t="s">
         <v>41</v>
       </c>
+      <c r="H17" s="107"/>
     </row>
     <row r="18" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="22" t="s">
-        <v>84</v>
-      </c>
       <c r="B18" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="D18" s="33" t="s">
+      <c r="C18" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" s="52" t="s">
         <v>154</v>
       </c>
-      <c r="E18" s="36" t="s">
+      <c r="E18" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="F18" s="36" t="s">
+      <c r="F18" s="32" t="s">
         <v>176</v>
       </c>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
     </row>
     <row r="19" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="22" t="s">
-        <v>84</v>
-      </c>
       <c r="B19" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="D19" s="33" t="s">
+      <c r="C19" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="52" t="s">
         <v>154</v>
       </c>
-      <c r="E19" s="33" t="s">
+      <c r="E19" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="33" t="s">
+      <c r="F19" s="52" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="22" t="s">
-        <v>84</v>
-      </c>
       <c r="B20" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="D20" s="33" t="s">
+      <c r="C20" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" s="52" t="s">
         <v>154</v>
       </c>
-      <c r="E20" s="33" t="s">
+      <c r="E20" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="F20" s="33" t="s">
+      <c r="F20" s="52" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="22" t="s">
-        <v>84</v>
-      </c>
       <c r="B21" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="D21" s="33" t="s">
+      <c r="C21" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" s="52" t="s">
         <v>154</v>
       </c>
-      <c r="E21" s="33" t="s">
+      <c r="E21" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="F21" s="33" t="s">
+      <c r="F21" s="52" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="22" t="s">
-        <v>84</v>
-      </c>
       <c r="B22" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="D22" s="33" t="s">
+      <c r="C22" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="D22" s="52" t="s">
         <v>154</v>
       </c>
-      <c r="E22" s="33" t="s">
+      <c r="E22" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="F22" s="33" t="s">
+      <c r="F22" s="52" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="23" t="s">
-        <v>84</v>
-      </c>
+      <c r="A23" s="23"/>
       <c r="B23" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="D23" s="35" t="s">
+      <c r="C23" s="55" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23" s="53" t="s">
         <v>154</v>
       </c>
-      <c r="E23" s="35" t="s">
+      <c r="E23" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="35" t="s">
+      <c r="F23" s="53" t="s">
         <v>181</v>
       </c>
       <c r="G23" s="23"/>
+      <c r="H23" s="103"/>
     </row>
     <row r="24" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="22" t="s">
-        <v>84</v>
-      </c>
       <c r="B24" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="C24" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="D24" s="34" t="s">
+      <c r="C24" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" s="51" t="s">
         <v>155</v>
       </c>
-      <c r="E24" s="36" t="s">
+      <c r="E24" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="F24" s="36" t="s">
-        <v>193</v>
-      </c>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42"/>
+      <c r="F24" s="32" t="s">
+        <v>308</v>
+      </c>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
     </row>
     <row r="25" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="22" t="s">
-        <v>84</v>
-      </c>
       <c r="B25" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="C25" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="D25" s="34" t="s">
+      <c r="C25" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="D25" s="51" t="s">
         <v>155</v>
       </c>
-      <c r="E25" s="34" t="s">
+      <c r="E25" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="F25" s="34" t="s">
-        <v>194</v>
+      <c r="F25" s="51" t="s">
+        <v>193</v>
       </c>
       <c r="G25" s="22" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="22" t="s">
-        <v>84</v>
-      </c>
       <c r="B26" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="C26" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="D26" s="34" t="s">
+      <c r="C26" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="D26" s="51" t="s">
         <v>155</v>
       </c>
-      <c r="E26" s="34" t="s">
+      <c r="E26" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="F26" s="34" t="s">
-        <v>195</v>
+      <c r="F26" s="51" t="s">
+        <v>194</v>
       </c>
       <c r="G26" s="22" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="22" t="s">
-        <v>84</v>
-      </c>
       <c r="B27" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="C27" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="D27" s="34" t="s">
+      <c r="C27" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27" s="51" t="s">
         <v>155</v>
       </c>
-      <c r="E27" s="34" t="s">
+      <c r="E27" s="51" t="s">
         <v>55</v>
       </c>
-      <c r="F27" s="34" t="s">
-        <v>196</v>
+      <c r="F27" s="51" t="s">
+        <v>195</v>
       </c>
       <c r="G27" s="22" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="107" t="s">
         <v>94</v>
       </c>
-      <c r="C28" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="D28" s="34" t="s">
+      <c r="C28" s="108" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" s="109" t="s">
         <v>155</v>
       </c>
-      <c r="E28" s="34" t="s">
+      <c r="E28" s="109" t="s">
         <v>57</v>
       </c>
-      <c r="F28" s="34" t="s">
-        <v>197</v>
-      </c>
-      <c r="G28" s="22" t="s">
+      <c r="F28" s="109" t="s">
+        <v>196</v>
+      </c>
+      <c r="G28" s="107" t="s">
         <v>58</v>
       </c>
+      <c r="H28" s="107"/>
     </row>
     <row r="29" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="22" t="s">
-        <v>84</v>
-      </c>
       <c r="B29" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="C29" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="D29" s="33" t="s">
+      <c r="C29" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="D29" s="52" t="s">
         <v>154</v>
       </c>
-      <c r="E29" s="36" t="s">
+      <c r="E29" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="F29" s="36" t="s">
+      <c r="F29" s="32" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="22" t="s">
-        <v>84</v>
-      </c>
       <c r="B30" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="C30" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="D30" s="33" t="s">
+      <c r="C30" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="D30" s="52" t="s">
         <v>154</v>
       </c>
-      <c r="E30" s="33" t="s">
+      <c r="E30" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="F30" s="33" t="s">
-        <v>198</v>
+      <c r="F30" s="52" t="s">
+        <v>197</v>
       </c>
       <c r="G30" s="22" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="22" t="s">
-        <v>84</v>
-      </c>
       <c r="B31" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="C31" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="D31" s="33" t="s">
+      <c r="C31" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="D31" s="52" t="s">
         <v>154</v>
       </c>
-      <c r="E31" s="33" t="s">
+      <c r="E31" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="F31" s="33" t="s">
-        <v>201</v>
+      <c r="F31" s="52" t="s">
+        <v>200</v>
       </c>
       <c r="G31" s="22" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="23" t="s">
+    <row r="32" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="71"/>
+      <c r="B32" s="71" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="72" t="s">
+        <v>92</v>
+      </c>
+      <c r="D32" s="74" t="s">
+        <v>154</v>
+      </c>
+      <c r="E32" s="74" t="s">
+        <v>64</v>
+      </c>
+      <c r="F32" s="74" t="s">
+        <v>175</v>
+      </c>
+      <c r="G32" s="71" t="s">
+        <v>65</v>
+      </c>
+      <c r="H32" s="71"/>
+    </row>
+    <row r="33" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="102" t="s">
+        <v>95</v>
+      </c>
+      <c r="B33" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="F33" s="38" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B34" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="67" t="s">
+        <v>76</v>
+      </c>
+      <c r="F34" s="22" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B35" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="67" t="s">
+        <v>77</v>
+      </c>
+      <c r="F35" s="22" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B36" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="67" t="s">
+        <v>78</v>
+      </c>
+      <c r="F36" s="22" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B37" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C37" s="105" t="s">
+        <v>92</v>
+      </c>
+      <c r="E37" s="70" t="s">
+        <v>71</v>
+      </c>
+      <c r="F37" s="38" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B38" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C38" s="105" t="s">
+        <v>92</v>
+      </c>
+      <c r="D38" s="52" t="s">
+        <v>154</v>
+      </c>
+      <c r="E38" s="69" t="s">
+        <v>79</v>
+      </c>
+      <c r="F38" s="52" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B39" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C39" s="105" t="s">
+        <v>92</v>
+      </c>
+      <c r="E39" s="67" t="s">
+        <v>80</v>
+      </c>
+      <c r="F39" s="22" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="71"/>
+      <c r="B40" s="71" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40" s="72" t="s">
+        <v>92</v>
+      </c>
+      <c r="D40" s="71"/>
+      <c r="E40" s="73" t="s">
+        <v>81</v>
+      </c>
+      <c r="F40" s="71" t="s">
+        <v>263</v>
+      </c>
+      <c r="G40" s="71"/>
+      <c r="H40" s="71"/>
+    </row>
+    <row r="41" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="102" t="s">
+        <v>231</v>
+      </c>
+      <c r="B41" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" s="75" t="s">
+        <v>70</v>
+      </c>
+      <c r="F41" s="84" t="s">
+        <v>269</v>
+      </c>
+      <c r="G41" s="93"/>
+      <c r="H41" s="93"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B42" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" s="64" t="s">
+        <v>76</v>
+      </c>
+      <c r="F42" s="22" t="s">
+        <v>265</v>
+      </c>
+      <c r="G42" s="66"/>
+      <c r="H42" s="93"/>
+    </row>
+    <row r="43" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B43" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" s="64" t="s">
+        <v>232</v>
+      </c>
+      <c r="F43" s="22" t="s">
+        <v>266</v>
+      </c>
+      <c r="G43" s="93"/>
+      <c r="H43" s="93"/>
+    </row>
+    <row r="44" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B44" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44" s="64" t="s">
+        <v>233</v>
+      </c>
+      <c r="F44" s="22" t="s">
+        <v>268</v>
+      </c>
+      <c r="G44" s="66"/>
+      <c r="H44" s="93"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B45" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C45" s="55" t="s">
+        <v>92</v>
+      </c>
+      <c r="E45" s="76" t="s">
+        <v>71</v>
+      </c>
+      <c r="F45" s="38" t="s">
+        <v>273</v>
+      </c>
+      <c r="G45" s="66"/>
+      <c r="H45" s="93"/>
+    </row>
+    <row r="46" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B46" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C46" s="55" t="s">
+        <v>92</v>
+      </c>
+      <c r="E46" s="64" t="s">
+        <v>234</v>
+      </c>
+      <c r="F46" s="22" t="s">
+        <v>270</v>
+      </c>
+      <c r="G46" s="66"/>
+      <c r="H46" s="93"/>
+    </row>
+    <row r="47" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B47" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C47" s="55" t="s">
+        <v>92</v>
+      </c>
+      <c r="E47" s="64" t="s">
+        <v>235</v>
+      </c>
+      <c r="F47" s="22" t="s">
+        <v>271</v>
+      </c>
+      <c r="G47" s="66"/>
+      <c r="H47" s="93"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B48" s="22" t="s">
+        <v>236</v>
+      </c>
+      <c r="C48" s="55" t="s">
+        <v>92</v>
+      </c>
+      <c r="D48" s="51" t="s">
+        <v>155</v>
+      </c>
+      <c r="E48" s="76" t="s">
+        <v>237</v>
+      </c>
+      <c r="F48" s="38" t="s">
+        <v>274</v>
+      </c>
+      <c r="G48" s="66"/>
+      <c r="H48" s="93"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B49" s="22" t="s">
+        <v>236</v>
+      </c>
+      <c r="C49" s="55" t="s">
+        <v>92</v>
+      </c>
+      <c r="D49" s="51" t="s">
+        <v>155</v>
+      </c>
+      <c r="E49" s="85" t="s">
+        <v>238</v>
+      </c>
+      <c r="F49" s="51" t="s">
+        <v>275</v>
+      </c>
+      <c r="G49" s="64" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="71"/>
+      <c r="B50" s="71" t="s">
+        <v>236</v>
+      </c>
+      <c r="C50" s="55" t="s">
+        <v>92</v>
+      </c>
+      <c r="D50" s="51" t="s">
+        <v>155</v>
+      </c>
+      <c r="E50" s="86" t="s">
+        <v>240</v>
+      </c>
+      <c r="F50" s="51" t="s">
+        <v>272</v>
+      </c>
+      <c r="G50" s="77" t="s">
+        <v>241</v>
+      </c>
+      <c r="H50" s="71"/>
+    </row>
+    <row r="51" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="101" t="s">
         <v>84</v>
       </c>
-      <c r="B32" s="23" t="s">
+      <c r="B51" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C51" s="91" t="s">
+        <v>226</v>
+      </c>
+      <c r="E51" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="F51" s="38" t="s">
+        <v>292</v>
+      </c>
+      <c r="G51" s="38"/>
+      <c r="H51" s="38" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B52" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C52" s="91" t="s">
+        <v>226</v>
+      </c>
+      <c r="E52" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="F52" s="22" t="s">
+        <v>293</v>
+      </c>
+      <c r="G52" s="22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B53" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C53" s="91" t="s">
+        <v>226</v>
+      </c>
+      <c r="E53" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="F53" s="22" t="s">
+        <v>294</v>
+      </c>
+      <c r="G53" s="22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B54" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C54" s="91" t="s">
+        <v>226</v>
+      </c>
+      <c r="D54" s="94" t="s">
+        <v>153</v>
+      </c>
+      <c r="E54" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="F54" s="38" t="s">
+        <v>295</v>
+      </c>
+      <c r="G54" s="38"/>
+      <c r="H54" s="38" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B55" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C55" s="91" t="s">
+        <v>226</v>
+      </c>
+      <c r="D55" s="94" t="s">
+        <v>153</v>
+      </c>
+      <c r="E55" s="94" t="s">
+        <v>32</v>
+      </c>
+      <c r="F55" s="94" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B56" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C56" s="91" t="s">
+        <v>226</v>
+      </c>
+      <c r="D56" s="94" t="s">
+        <v>153</v>
+      </c>
+      <c r="E56" s="94" t="s">
+        <v>33</v>
+      </c>
+      <c r="F56" s="94" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B57" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C57" s="91" t="s">
+        <v>226</v>
+      </c>
+      <c r="D57" s="94" t="s">
+        <v>153</v>
+      </c>
+      <c r="E57" s="94" t="s">
+        <v>34</v>
+      </c>
+      <c r="F57" s="94" t="s">
+        <v>298</v>
+      </c>
+      <c r="G57" s="22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B58" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C58" s="91" t="s">
+        <v>226</v>
+      </c>
+      <c r="D58" s="94" t="s">
+        <v>153</v>
+      </c>
+      <c r="E58" s="94" t="s">
+        <v>36</v>
+      </c>
+      <c r="F58" s="94" t="s">
+        <v>299</v>
+      </c>
+      <c r="G58" s="22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B59" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C59" s="91" t="s">
+        <v>226</v>
+      </c>
+      <c r="D59" s="94" t="s">
+        <v>153</v>
+      </c>
+      <c r="E59" s="94" t="s">
+        <v>38</v>
+      </c>
+      <c r="F59" s="94" t="s">
+        <v>300</v>
+      </c>
+      <c r="G59" s="22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B60" s="107" t="s">
+        <v>11</v>
+      </c>
+      <c r="C60" s="110" t="s">
+        <v>226</v>
+      </c>
+      <c r="D60" s="111" t="s">
+        <v>153</v>
+      </c>
+      <c r="E60" s="111" t="s">
+        <v>40</v>
+      </c>
+      <c r="F60" s="111" t="s">
+        <v>301</v>
+      </c>
+      <c r="G60" s="107" t="s">
+        <v>41</v>
+      </c>
+      <c r="H60" s="107"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B61" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C61" s="91" t="s">
+        <v>226</v>
+      </c>
+      <c r="D61" s="97" t="s">
+        <v>154</v>
+      </c>
+      <c r="E61" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="F61" s="38" t="s">
+        <v>302</v>
+      </c>
+      <c r="G61" s="38"/>
+      <c r="H61" s="38"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B62" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C62" s="91" t="s">
+        <v>226</v>
+      </c>
+      <c r="D62" s="97" t="s">
+        <v>154</v>
+      </c>
+      <c r="E62" s="97" t="s">
+        <v>18</v>
+      </c>
+      <c r="F62" s="97" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B63" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C63" s="91" t="s">
+        <v>226</v>
+      </c>
+      <c r="D63" s="97" t="s">
+        <v>154</v>
+      </c>
+      <c r="E63" s="97" t="s">
+        <v>19</v>
+      </c>
+      <c r="F63" s="97" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B64" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C64" s="91" t="s">
+        <v>226</v>
+      </c>
+      <c r="D64" s="97" t="s">
+        <v>154</v>
+      </c>
+      <c r="E64" s="97" t="s">
+        <v>20</v>
+      </c>
+      <c r="F64" s="97" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B65" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C65" s="91" t="s">
+        <v>226</v>
+      </c>
+      <c r="D65" s="97" t="s">
+        <v>154</v>
+      </c>
+      <c r="E65" s="97" t="s">
+        <v>21</v>
+      </c>
+      <c r="F65" s="97" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A66" s="23"/>
+      <c r="B66" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C66" s="104" t="s">
+        <v>226</v>
+      </c>
+      <c r="D66" s="100" t="s">
+        <v>154</v>
+      </c>
+      <c r="E66" s="100" t="s">
+        <v>22</v>
+      </c>
+      <c r="F66" s="100" t="s">
+        <v>307</v>
+      </c>
+      <c r="G66" s="23"/>
+      <c r="H66" s="103"/>
+    </row>
+    <row r="67" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B67" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="C32" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="D32" s="35" t="s">
+      <c r="C67" s="91" t="s">
+        <v>226</v>
+      </c>
+      <c r="D67" s="94" t="s">
+        <v>155</v>
+      </c>
+      <c r="E67" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="F67" s="38" t="s">
+        <v>309</v>
+      </c>
+      <c r="G67" s="38"/>
+    </row>
+    <row r="68" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B68" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="C68" s="91" t="s">
+        <v>226</v>
+      </c>
+      <c r="D68" s="94" t="s">
+        <v>155</v>
+      </c>
+      <c r="E68" s="94" t="s">
+        <v>51</v>
+      </c>
+      <c r="F68" s="94" t="s">
+        <v>310</v>
+      </c>
+      <c r="G68" s="22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B69" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="C69" s="91" t="s">
+        <v>226</v>
+      </c>
+      <c r="D69" s="94" t="s">
+        <v>155</v>
+      </c>
+      <c r="E69" s="94" t="s">
+        <v>53</v>
+      </c>
+      <c r="F69" s="94" t="s">
+        <v>311</v>
+      </c>
+      <c r="G69" s="22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B70" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="C70" s="91" t="s">
+        <v>226</v>
+      </c>
+      <c r="D70" s="94" t="s">
+        <v>155</v>
+      </c>
+      <c r="E70" s="94" t="s">
+        <v>55</v>
+      </c>
+      <c r="F70" s="94" t="s">
+        <v>312</v>
+      </c>
+      <c r="G70" s="22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B71" s="107" t="s">
+        <v>94</v>
+      </c>
+      <c r="C71" s="110" t="s">
+        <v>226</v>
+      </c>
+      <c r="D71" s="111" t="s">
+        <v>155</v>
+      </c>
+      <c r="E71" s="111" t="s">
+        <v>57</v>
+      </c>
+      <c r="F71" s="111" t="s">
+        <v>313</v>
+      </c>
+      <c r="G71" s="107" t="s">
+        <v>58</v>
+      </c>
+      <c r="H71" s="107"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B72" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="C72" s="91" t="s">
+        <v>226</v>
+      </c>
+      <c r="D72" s="97" t="s">
         <v>154</v>
       </c>
-      <c r="E32" s="35" t="s">
+      <c r="E72" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="F72" s="38" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B73" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="C73" s="91" t="s">
+        <v>226</v>
+      </c>
+      <c r="D73" s="97" t="s">
+        <v>154</v>
+      </c>
+      <c r="E73" s="97" t="s">
+        <v>60</v>
+      </c>
+      <c r="F73" s="97" t="s">
+        <v>315</v>
+      </c>
+      <c r="G73" s="22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B74" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="C74" s="91" t="s">
+        <v>226</v>
+      </c>
+      <c r="D74" s="97" t="s">
+        <v>154</v>
+      </c>
+      <c r="E74" s="97" t="s">
+        <v>62</v>
+      </c>
+      <c r="F74" s="97" t="s">
+        <v>316</v>
+      </c>
+      <c r="G74" s="22" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="71"/>
+      <c r="B75" s="71" t="s">
+        <v>94</v>
+      </c>
+      <c r="C75" s="91" t="s">
+        <v>226</v>
+      </c>
+      <c r="D75" s="98" t="s">
+        <v>154</v>
+      </c>
+      <c r="E75" s="98" t="s">
         <v>64</v>
       </c>
-      <c r="F32" s="35" t="s">
-        <v>175</v>
-      </c>
-      <c r="G32" s="23" t="s">
+      <c r="F75" s="98" t="s">
+        <v>314</v>
+      </c>
+      <c r="G75" s="71" t="s">
         <v>65</v>
       </c>
-      <c r="H32" s="43"/>
+      <c r="H75" s="71"/>
+    </row>
+    <row r="76" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="102" t="s">
+        <v>95</v>
+      </c>
+      <c r="B76" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C76" s="91" t="s">
+        <v>226</v>
+      </c>
+      <c r="E76" s="70" t="s">
+        <v>71</v>
+      </c>
+      <c r="F76" s="38" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B77" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C77" s="91" t="s">
+        <v>226</v>
+      </c>
+      <c r="D77" s="97" t="s">
+        <v>154</v>
+      </c>
+      <c r="E77" s="68" t="s">
+        <v>79</v>
+      </c>
+      <c r="F77" s="97" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="B78" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C78" s="91" t="s">
+        <v>226</v>
+      </c>
+      <c r="E78" s="67" t="s">
+        <v>80</v>
+      </c>
+      <c r="F78" s="22" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="71"/>
+      <c r="B79" s="71" t="s">
+        <v>85</v>
+      </c>
+      <c r="C79" s="91" t="s">
+        <v>226</v>
+      </c>
+      <c r="D79" s="71"/>
+      <c r="E79" s="73" t="s">
+        <v>81</v>
+      </c>
+      <c r="F79" s="71" t="s">
+        <v>320</v>
+      </c>
+      <c r="G79" s="71"/>
+      <c r="H79" s="71"/>
+    </row>
+    <row r="80" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="102" t="s">
+        <v>231</v>
+      </c>
+      <c r="B80" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C80" s="91" t="s">
+        <v>226</v>
+      </c>
+      <c r="E80" s="76" t="s">
+        <v>71</v>
+      </c>
+      <c r="F80" s="38" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B81" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C81" s="91" t="s">
+        <v>226</v>
+      </c>
+      <c r="E81" s="64" t="s">
+        <v>234</v>
+      </c>
+      <c r="F81" s="22" t="s">
+        <v>322</v>
+      </c>
+      <c r="G81" s="65"/>
+    </row>
+    <row r="82" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A82" s="103"/>
+      <c r="B82" s="103" t="s">
+        <v>85</v>
+      </c>
+      <c r="C82" s="104" t="s">
+        <v>226</v>
+      </c>
+      <c r="D82" s="103"/>
+      <c r="E82" s="112" t="s">
+        <v>235</v>
+      </c>
+      <c r="F82" s="103" t="s">
+        <v>323</v>
+      </c>
+      <c r="G82" s="113"/>
+      <c r="H82" s="103"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B83" s="22" t="s">
+        <v>236</v>
+      </c>
+      <c r="C83" s="91" t="s">
+        <v>226</v>
+      </c>
+      <c r="D83" s="94" t="s">
+        <v>155</v>
+      </c>
+      <c r="E83" s="76" t="s">
+        <v>237</v>
+      </c>
+      <c r="F83" s="38" t="s">
+        <v>324</v>
+      </c>
+      <c r="G83" s="65"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B84" s="22" t="s">
+        <v>236</v>
+      </c>
+      <c r="C84" s="91" t="s">
+        <v>226</v>
+      </c>
+      <c r="D84" s="94" t="s">
+        <v>155</v>
+      </c>
+      <c r="E84" s="95" t="s">
+        <v>238</v>
+      </c>
+      <c r="F84" s="94" t="s">
+        <v>325</v>
+      </c>
+      <c r="G84" s="64" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="71"/>
+      <c r="B85" s="71" t="s">
+        <v>236</v>
+      </c>
+      <c r="C85" s="92" t="s">
+        <v>226</v>
+      </c>
+      <c r="D85" s="99" t="s">
+        <v>155</v>
+      </c>
+      <c r="E85" s="96" t="s">
+        <v>240</v>
+      </c>
+      <c r="F85" s="99" t="s">
+        <v>326</v>
+      </c>
+      <c r="G85" s="77" t="s">
+        <v>241</v>
+      </c>
+      <c r="H85" s="71"/>
+    </row>
+    <row r="86" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="G86" s="65"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="G87" s="65"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A89" s="93"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41:D50"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3057,10 +5928,10 @@
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="B12" s="44"/>
+      <c r="B12" s="39"/>
       <c r="C12" s="12" t="s">
         <v>32</v>
       </c>
@@ -3121,10 +5992,10 @@
       <c r="D18" s="11"/>
     </row>
     <row r="19" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="44" t="s">
+      <c r="A19" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="B19" s="44"/>
+      <c r="B19" s="39"/>
       <c r="C19" s="10" t="s">
         <v>18</v>
       </c>
@@ -3173,10 +6044,10 @@
       <c r="D24" s="12"/>
     </row>
     <row r="25" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="44" t="s">
+      <c r="A25" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="B25" s="44"/>
+      <c r="B25" s="39"/>
       <c r="C25" s="10" t="s">
         <v>51</v>
       </c>
@@ -3223,10 +6094,10 @@
       <c r="D29" s="6"/>
     </row>
     <row r="30" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="44" t="s">
+      <c r="A30" s="39" t="s">
         <v>93</v>
       </c>
-      <c r="B30" s="44"/>
+      <c r="B30" s="39"/>
       <c r="C30" s="12" t="s">
         <v>60</v>
       </c>
@@ -3322,6 +6193,98 @@
         <v>81</v>
       </c>
       <c r="D40" s="9"/>
+    </row>
+    <row r="41" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" s="60" t="s">
+        <v>70</v>
+      </c>
+      <c r="D41" s="17"/>
+    </row>
+    <row r="42" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="18"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D42" s="12"/>
+    </row>
+    <row r="43" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="18"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="D43" s="2"/>
+    </row>
+    <row r="44" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="18"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="D44" s="12"/>
+    </row>
+    <row r="45" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="2"/>
+      <c r="B45" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D45" s="2"/>
+    </row>
+    <row r="46" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="18"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="D46" s="12"/>
+    </row>
+    <row r="47" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="18"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="D47" s="2"/>
+    </row>
+    <row r="48" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="18"/>
+      <c r="B48" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="D48" s="12"/>
+    </row>
+    <row r="49" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="18"/>
+      <c r="B49" s="18"/>
+      <c r="C49" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>241</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
fix - Joint pattern detection. wrong regex
</commit_message>
<xml_diff>
--- a/Data/jointPatterns/Nieuwenhuys2017.xlsx
+++ b/Data/jointPatterns/Nieuwenhuys2017.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="328">
   <si>
     <t>Plan</t>
   </si>
@@ -364,9 +364,6 @@
   </si>
   <si>
     <t>decrease,normal,increase</t>
-  </si>
-  <si>
-    <t>Insufficient,normal,excessive</t>
   </si>
   <si>
     <t>-5,5</t>
@@ -1105,6 +1102,12 @@
   </si>
   <si>
     <t>#61[insufficient]</t>
+  </si>
+  <si>
+    <t>increase,normal,decrease</t>
+  </si>
+  <si>
+    <t>excessive,normal,</t>
   </si>
 </sst>
 </file>
@@ -1468,9 +1471,6 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1680,6 +1680,9 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1986,8 +1989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H60" sqref="H60"/>
+    <sheetView tabSelected="1" topLeftCell="C22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2002,7 +2005,7 @@
     <col min="9" max="9" width="21.6640625" style="1" customWidth="1"/>
     <col min="10" max="10" width="16.88671875" style="1" customWidth="1"/>
     <col min="11" max="11" width="18.44140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="15.44140625" style="63" customWidth="1"/>
+    <col min="12" max="12" width="15.44140625" style="62" customWidth="1"/>
     <col min="13" max="13" width="46.6640625" style="1" customWidth="1"/>
     <col min="14" max="16384" width="8.88671875" style="1"/>
   </cols>
@@ -2045,7 +2048,7 @@
         <v>101</v>
       </c>
       <c r="M1" s="24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -2081,7 +2084,7 @@
       </c>
       <c r="K2" s="25"/>
       <c r="L2" s="34" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M2" s="25"/>
     </row>
@@ -2096,7 +2099,7 @@
         <v>115</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E3" s="26" t="s">
         <v>92</v>
@@ -2118,21 +2121,21 @@
       </c>
       <c r="K3" s="26"/>
       <c r="L3" s="35" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="M3" s="26"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="47">
+      <c r="A4" s="46">
         <v>3</v>
       </c>
       <c r="B4" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>115</v>
-      </c>
-      <c r="D4" s="43" t="s">
+        <v>326</v>
+      </c>
+      <c r="D4" s="42" t="s">
         <v>49</v>
       </c>
       <c r="E4" s="25" t="s">
@@ -2147,7 +2150,7 @@
       <c r="H4" s="25">
         <v>0</v>
       </c>
-      <c r="I4" s="43" t="s">
+      <c r="I4" s="42" t="s">
         <v>89</v>
       </c>
       <c r="J4" s="25" t="s">
@@ -2155,12 +2158,12 @@
       </c>
       <c r="K4" s="25"/>
       <c r="L4" s="34" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M4" s="25"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="47">
+      <c r="A5" s="46">
         <v>4</v>
       </c>
       <c r="B5" s="25" t="s">
@@ -2169,7 +2172,7 @@
       <c r="C5" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="D5" s="43" t="s">
+      <c r="D5" s="42" t="s">
         <v>75</v>
       </c>
       <c r="E5" s="25" t="s">
@@ -2184,7 +2187,7 @@
       <c r="H5" s="25">
         <v>0</v>
       </c>
-      <c r="I5" s="43" t="s">
+      <c r="I5" s="42" t="s">
         <v>89</v>
       </c>
       <c r="J5" s="25" t="s">
@@ -2192,12 +2195,12 @@
       </c>
       <c r="K5" s="25"/>
       <c r="L5" s="34" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="M5" s="25"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="48">
+      <c r="A6" s="47">
         <v>5</v>
       </c>
       <c r="B6" s="27" t="s">
@@ -2206,7 +2209,7 @@
       <c r="C6" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="D6" s="44" t="s">
+      <c r="D6" s="43" t="s">
         <v>111</v>
       </c>
       <c r="E6" s="27" t="s">
@@ -2221,7 +2224,7 @@
       <c r="H6" s="25">
         <v>0</v>
       </c>
-      <c r="I6" s="43" t="s">
+      <c r="I6" s="42" t="s">
         <v>89</v>
       </c>
       <c r="J6" s="25" t="s">
@@ -2231,21 +2234,21 @@
         <v>0</v>
       </c>
       <c r="L6" s="34" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="M6" s="25"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="48">
+      <c r="A7" s="47">
         <v>6</v>
       </c>
       <c r="B7" s="27" t="s">
         <v>103</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>115</v>
-      </c>
-      <c r="D7" s="44" t="s">
+        <v>326</v>
+      </c>
+      <c r="D7" s="43" t="s">
         <v>44</v>
       </c>
       <c r="E7" s="27" t="s">
@@ -2260,7 +2263,7 @@
       <c r="H7" s="25">
         <v>0</v>
       </c>
-      <c r="I7" s="43" t="s">
+      <c r="I7" s="42" t="s">
         <v>89</v>
       </c>
       <c r="J7" s="25" t="s">
@@ -2268,12 +2271,12 @@
       </c>
       <c r="K7" s="25"/>
       <c r="L7" s="34" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="M7" s="25"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="47">
+      <c r="A8" s="46">
         <v>7</v>
       </c>
       <c r="B8" s="25" t="s">
@@ -2302,13 +2305,13 @@
         <v>69</v>
       </c>
       <c r="K8" s="25" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L8" s="34"/>
       <c r="M8" s="25"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="49">
+      <c r="A9" s="48">
         <v>8</v>
       </c>
       <c r="B9" s="26" t="s">
@@ -2337,13 +2340,13 @@
         <v>69</v>
       </c>
       <c r="K9" s="26" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L9" s="35"/>
       <c r="M9" s="26"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="47">
+      <c r="A10" s="46">
         <v>9</v>
       </c>
       <c r="B10" s="25" t="s">
@@ -2377,12 +2380,12 @@
         <v>0</v>
       </c>
       <c r="L10" s="34" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M10" s="25"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="47">
+      <c r="A11" s="46">
         <v>10</v>
       </c>
       <c r="B11" s="25" t="s">
@@ -2391,8 +2394,8 @@
       <c r="C11" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="D11" s="43" t="s">
-        <v>187</v>
+      <c r="D11" s="42" t="s">
+        <v>186</v>
       </c>
       <c r="E11" s="25" t="s">
         <v>92</v>
@@ -2406,7 +2409,7 @@
       <c r="H11" s="25">
         <v>0</v>
       </c>
-      <c r="I11" s="43" t="s">
+      <c r="I11" s="42" t="s">
         <v>89</v>
       </c>
       <c r="J11" s="25" t="s">
@@ -2414,19 +2417,19 @@
       </c>
       <c r="K11" s="25"/>
       <c r="L11" s="34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M11" s="25"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="48" t="s">
-        <v>186</v>
+      <c r="A12" s="47" t="s">
+        <v>185</v>
       </c>
       <c r="B12" s="27" t="s">
         <v>103</v>
       </c>
       <c r="C12" s="27"/>
-      <c r="D12" s="44" t="s">
+      <c r="D12" s="43" t="s">
         <v>112</v>
       </c>
       <c r="E12" s="27" t="s">
@@ -2441,27 +2444,27 @@
       <c r="H12" s="25">
         <v>0</v>
       </c>
-      <c r="I12" s="43" t="s">
+      <c r="I12" s="42" t="s">
         <v>89</v>
       </c>
       <c r="J12" s="25" t="s">
         <v>69</v>
       </c>
       <c r="K12" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L12" s="34"/>
       <c r="M12" s="25"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="48" t="s">
-        <v>166</v>
+      <c r="A13" s="47" t="s">
+        <v>165</v>
       </c>
       <c r="B13" s="27" t="s">
         <v>103</v>
       </c>
       <c r="C13" s="27"/>
-      <c r="D13" s="44" t="s">
+      <c r="D13" s="43" t="s">
         <v>17</v>
       </c>
       <c r="E13" s="27" t="s">
@@ -2476,29 +2479,29 @@
       <c r="H13" s="25">
         <v>0</v>
       </c>
-      <c r="I13" s="43" t="s">
+      <c r="I13" s="42" t="s">
         <v>89</v>
       </c>
       <c r="J13" s="25" t="s">
         <v>69</v>
       </c>
       <c r="K13" s="25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L13" s="34"/>
       <c r="M13" s="25"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="47" t="s">
-        <v>167</v>
+      <c r="A14" s="46" t="s">
+        <v>166</v>
       </c>
       <c r="B14" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>115</v>
-      </c>
-      <c r="D14" s="42" t="s">
+        <v>326</v>
+      </c>
+      <c r="D14" s="41" t="s">
         <v>47</v>
       </c>
       <c r="E14" s="25" t="s">
@@ -2513,29 +2516,29 @@
       <c r="H14" s="25">
         <v>0</v>
       </c>
-      <c r="I14" s="42" t="s">
-        <v>137</v>
+      <c r="I14" s="41" t="s">
+        <v>136</v>
       </c>
       <c r="J14" s="25" t="s">
         <v>6</v>
       </c>
       <c r="K14" s="25"/>
       <c r="L14" s="34" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M14" s="25"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="48" t="s">
-        <v>168</v>
+      <c r="A15" s="47" t="s">
+        <v>167</v>
       </c>
       <c r="B15" s="27" t="s">
         <v>103</v>
       </c>
       <c r="C15" s="27" t="s">
-        <v>116</v>
-      </c>
-      <c r="D15" s="45" t="s">
+        <v>249</v>
+      </c>
+      <c r="D15" s="44" t="s">
         <v>107</v>
       </c>
       <c r="E15" s="27" t="s">
@@ -2550,21 +2553,21 @@
       <c r="H15" s="25">
         <v>0</v>
       </c>
-      <c r="I15" s="42" t="s">
-        <v>137</v>
+      <c r="I15" s="41" t="s">
+        <v>136</v>
       </c>
       <c r="J15" s="25" t="s">
         <v>6</v>
       </c>
       <c r="K15" s="25"/>
       <c r="L15" s="34" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M15" s="25"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="47" t="s">
-        <v>169</v>
+      <c r="A16" s="46" t="s">
+        <v>168</v>
       </c>
       <c r="B16" s="25" t="s">
         <v>13</v>
@@ -2572,7 +2575,7 @@
       <c r="C16" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="D16" s="42" t="s">
+      <c r="D16" s="41" t="s">
         <v>108</v>
       </c>
       <c r="E16" s="25" t="s">
@@ -2587,21 +2590,21 @@
       <c r="H16" s="25">
         <v>0</v>
       </c>
-      <c r="I16" s="42" t="s">
-        <v>136</v>
+      <c r="I16" s="41" t="s">
+        <v>135</v>
       </c>
       <c r="J16" s="25" t="s">
         <v>7</v>
       </c>
       <c r="K16" s="25"/>
       <c r="L16" s="34" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M16" s="25"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="47" t="s">
-        <v>170</v>
+      <c r="A17" s="46" t="s">
+        <v>169</v>
       </c>
       <c r="B17" s="25" t="s">
         <v>13</v>
@@ -2609,7 +2612,7 @@
       <c r="C17" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="D17" s="41" t="s">
+      <c r="D17" s="40" t="s">
         <v>48</v>
       </c>
       <c r="E17" s="25" t="s">
@@ -2624,7 +2627,7 @@
       <c r="H17" s="25">
         <v>0</v>
       </c>
-      <c r="I17" s="41" t="s">
+      <c r="I17" s="40" t="s">
         <v>90</v>
       </c>
       <c r="J17" s="25" t="s">
@@ -2632,13 +2635,13 @@
       </c>
       <c r="K17" s="25"/>
       <c r="L17" s="34" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M17" s="25"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="49" t="s">
-        <v>171</v>
+      <c r="A18" s="48" t="s">
+        <v>170</v>
       </c>
       <c r="B18" s="26" t="s">
         <v>13</v>
@@ -2646,7 +2649,7 @@
       <c r="C18" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="D18" s="46" t="s">
+      <c r="D18" s="45" t="s">
         <v>48</v>
       </c>
       <c r="E18" s="26" t="s">
@@ -2661,7 +2664,7 @@
       <c r="H18" s="26">
         <v>0</v>
       </c>
-      <c r="I18" s="46" t="s">
+      <c r="I18" s="45" t="s">
         <v>90</v>
       </c>
       <c r="J18" s="26" t="s">
@@ -2669,19 +2672,19 @@
       </c>
       <c r="K18" s="26"/>
       <c r="L18" s="35" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="M18" s="26"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="47" t="s">
-        <v>172</v>
+      <c r="A19" s="46" t="s">
+        <v>171</v>
       </c>
       <c r="B19" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>116</v>
+        <v>327</v>
       </c>
       <c r="D19" s="25" t="s">
         <v>67</v>
@@ -2708,19 +2711,19 @@
         <v>100</v>
       </c>
       <c r="L19" s="34" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M19" s="25"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="47" t="s">
-        <v>173</v>
+      <c r="A20" s="46" t="s">
+        <v>172</v>
       </c>
       <c r="B20" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C20" s="25"/>
-      <c r="D20" s="43" t="s">
+      <c r="D20" s="42" t="s">
         <v>66</v>
       </c>
       <c r="E20" s="25" t="s">
@@ -2735,28 +2738,28 @@
       <c r="H20" s="25">
         <v>0</v>
       </c>
-      <c r="I20" s="43" t="s">
+      <c r="I20" s="42" t="s">
         <v>89</v>
       </c>
       <c r="J20" s="25" t="s">
         <v>96</v>
       </c>
       <c r="K20" s="25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L20" s="34"/>
       <c r="M20" s="25"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="47" t="s">
-        <v>174</v>
+      <c r="A21" s="46" t="s">
+        <v>173</v>
       </c>
       <c r="B21" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C21" s="25"/>
-      <c r="D21" s="43" t="s">
-        <v>132</v>
+      <c r="D21" s="42" t="s">
+        <v>131</v>
       </c>
       <c r="E21" s="25" t="s">
         <v>92</v>
@@ -2765,32 +2768,32 @@
         <v>99</v>
       </c>
       <c r="G21" s="25" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H21" s="25">
         <v>0</v>
       </c>
-      <c r="I21" s="43" t="s">
+      <c r="I21" s="42" t="s">
         <v>89</v>
       </c>
       <c r="J21" s="25" t="s">
         <v>69</v>
       </c>
       <c r="K21" s="25" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L21" s="34"/>
       <c r="M21" s="25"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="47" t="s">
-        <v>144</v>
+      <c r="A22" s="46" t="s">
+        <v>143</v>
       </c>
       <c r="B22" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C22" s="25"/>
-      <c r="D22" s="43" t="s">
+      <c r="D22" s="42" t="s">
         <v>74</v>
       </c>
       <c r="E22" s="25" t="s">
@@ -2805,21 +2808,21 @@
       <c r="H22" s="25">
         <v>0</v>
       </c>
-      <c r="I22" s="43" t="s">
+      <c r="I22" s="42" t="s">
         <v>89</v>
       </c>
       <c r="J22" s="25" t="s">
         <v>69</v>
       </c>
       <c r="K22" s="25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L22" s="34"/>
       <c r="M22" s="25"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="47" t="s">
-        <v>145</v>
+      <c r="A23" s="46" t="s">
+        <v>144</v>
       </c>
       <c r="B23" s="25" t="s">
         <v>13</v>
@@ -2827,7 +2830,7 @@
       <c r="C23" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="D23" s="42" t="s">
+      <c r="D23" s="41" t="s">
         <v>109</v>
       </c>
       <c r="E23" s="25" t="s">
@@ -2837,26 +2840,26 @@
         <v>99</v>
       </c>
       <c r="G23" s="25" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H23" s="25">
         <v>0</v>
       </c>
-      <c r="I23" s="42" t="s">
-        <v>143</v>
+      <c r="I23" s="41" t="s">
+        <v>142</v>
       </c>
       <c r="J23" s="25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K23" s="25"/>
       <c r="L23" s="34" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M23" s="25"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="47" t="s">
-        <v>146</v>
+      <c r="A24" s="46" t="s">
+        <v>145</v>
       </c>
       <c r="B24" s="25" t="s">
         <v>13</v>
@@ -2864,7 +2867,7 @@
       <c r="C24" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="D24" s="41" t="s">
+      <c r="D24" s="40" t="s">
         <v>87</v>
       </c>
       <c r="E24" s="25" t="s">
@@ -2879,65 +2882,65 @@
       <c r="H24" s="25">
         <v>0</v>
       </c>
-      <c r="I24" s="41" t="s">
+      <c r="I24" s="40" t="s">
         <v>90</v>
       </c>
       <c r="J24" s="25" t="s">
         <v>69</v>
       </c>
       <c r="K24" s="25" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="L24" s="34"/>
       <c r="M24" s="25"/>
     </row>
-    <row r="25" spans="1:13" s="40" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="78" t="s">
-        <v>199</v>
-      </c>
-      <c r="B25" s="79" t="s">
+    <row r="25" spans="1:13" s="39" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="77" t="s">
+        <v>198</v>
+      </c>
+      <c r="B25" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="80"/>
-      <c r="D25" s="81" t="s">
-        <v>198</v>
-      </c>
-      <c r="E25" s="79" t="s">
-        <v>92</v>
-      </c>
-      <c r="F25" s="79" t="s">
+      <c r="C25" s="79"/>
+      <c r="D25" s="80" t="s">
+        <v>197</v>
+      </c>
+      <c r="E25" s="78" t="s">
+        <v>92</v>
+      </c>
+      <c r="F25" s="78" t="s">
         <v>99</v>
       </c>
-      <c r="G25" s="79">
-        <v>0</v>
-      </c>
-      <c r="H25" s="79">
-        <v>0</v>
-      </c>
-      <c r="I25" s="81" t="s">
+      <c r="G25" s="78">
+        <v>0</v>
+      </c>
+      <c r="H25" s="78">
+        <v>0</v>
+      </c>
+      <c r="I25" s="80" t="s">
         <v>90</v>
       </c>
-      <c r="J25" s="79" t="s">
+      <c r="J25" s="78" t="s">
         <v>69</v>
       </c>
-      <c r="K25" s="79" t="s">
-        <v>141</v>
-      </c>
-      <c r="L25" s="82"/>
-      <c r="M25" s="80"/>
-    </row>
-    <row r="26" spans="1:13" s="58" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="56" t="s">
-        <v>203</v>
+      <c r="K25" s="78" t="s">
+        <v>140</v>
+      </c>
+      <c r="L25" s="81"/>
+      <c r="M25" s="79"/>
+    </row>
+    <row r="26" spans="1:13" s="57" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="55" t="s">
+        <v>202</v>
       </c>
       <c r="B26" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="57" t="s">
+      <c r="C26" s="56" t="s">
         <v>115</v>
       </c>
-      <c r="D26" s="59" t="s">
-        <v>242</v>
+      <c r="D26" s="58" t="s">
+        <v>241</v>
       </c>
       <c r="E26" s="34" t="s">
         <v>92</v>
@@ -2945,11 +2948,11 @@
       <c r="F26" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="G26" s="57" t="s">
-        <v>134</v>
-      </c>
-      <c r="H26" s="57" t="s">
-        <v>243</v>
+      <c r="G26" s="56" t="s">
+        <v>133</v>
+      </c>
+      <c r="H26" s="56" t="s">
+        <v>242</v>
       </c>
       <c r="I26" s="34" t="s">
         <v>46</v>
@@ -2957,20 +2960,20 @@
       <c r="J26" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="K26" s="57"/>
-      <c r="L26" s="61" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" s="58" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="56" t="s">
-        <v>204</v>
+      <c r="K26" s="56"/>
+      <c r="L26" s="60" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="55" t="s">
+        <v>203</v>
       </c>
       <c r="B27" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="59" t="s">
-        <v>246</v>
+      <c r="D27" s="58" t="s">
+        <v>245</v>
       </c>
       <c r="E27" s="34" t="s">
         <v>92</v>
@@ -2978,11 +2981,11 @@
       <c r="F27" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="G27" s="57" t="s">
-        <v>134</v>
-      </c>
-      <c r="H27" s="57" t="s">
-        <v>243</v>
+      <c r="G27" s="56" t="s">
+        <v>133</v>
+      </c>
+      <c r="H27" s="56" t="s">
+        <v>242</v>
       </c>
       <c r="I27" s="34" t="s">
         <v>46</v>
@@ -2991,19 +2994,19 @@
         <v>69</v>
       </c>
       <c r="K27" s="34" t="s">
-        <v>139</v>
-      </c>
-      <c r="L27" s="62"/>
-    </row>
-    <row r="28" spans="1:13" s="58" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="56" t="s">
-        <v>205</v>
+        <v>138</v>
+      </c>
+      <c r="L27" s="61"/>
+    </row>
+    <row r="28" spans="1:13" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="55" t="s">
+        <v>204</v>
       </c>
       <c r="B28" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="59" t="s">
-        <v>257</v>
+      <c r="D28" s="58" t="s">
+        <v>256</v>
       </c>
       <c r="E28" s="34" t="s">
         <v>92</v>
@@ -3011,11 +3014,11 @@
       <c r="F28" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="G28" s="57" t="s">
-        <v>134</v>
-      </c>
-      <c r="H28" s="57" t="s">
-        <v>243</v>
+      <c r="G28" s="56" t="s">
+        <v>133</v>
+      </c>
+      <c r="H28" s="56" t="s">
+        <v>242</v>
       </c>
       <c r="I28" s="34" t="s">
         <v>46</v>
@@ -3024,22 +3027,22 @@
         <v>69</v>
       </c>
       <c r="K28" s="34" t="s">
-        <v>142</v>
-      </c>
-      <c r="L28" s="62"/>
-    </row>
-    <row r="29" spans="1:13" s="58" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="56" t="s">
-        <v>206</v>
+        <v>141</v>
+      </c>
+      <c r="L28" s="61"/>
+    </row>
+    <row r="29" spans="1:13" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="55" t="s">
+        <v>205</v>
       </c>
       <c r="B29" s="34" t="s">
         <v>13</v>
       </c>
       <c r="C29" s="34" t="s">
-        <v>250</v>
-      </c>
-      <c r="D29" s="59" t="s">
-        <v>245</v>
+        <v>249</v>
+      </c>
+      <c r="D29" s="58" t="s">
+        <v>244</v>
       </c>
       <c r="E29" s="34" t="s">
         <v>92</v>
@@ -3047,151 +3050,151 @@
       <c r="F29" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="G29" s="57" t="s">
-        <v>134</v>
-      </c>
-      <c r="H29" s="57" t="s">
-        <v>243</v>
-      </c>
-      <c r="I29" s="41" t="s">
+      <c r="G29" s="56" t="s">
+        <v>133</v>
+      </c>
+      <c r="H29" s="56" t="s">
+        <v>242</v>
+      </c>
+      <c r="I29" s="40" t="s">
         <v>90</v>
       </c>
-      <c r="J29" s="57" t="s">
+      <c r="J29" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="K29" s="57"/>
-      <c r="L29" s="62" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" s="58" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="56" t="s">
-        <v>207</v>
+      <c r="K29" s="56"/>
+      <c r="L29" s="61" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="55" t="s">
+        <v>206</v>
       </c>
       <c r="B30" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="D30" s="59" t="s">
+      <c r="D30" s="58" t="s">
         <v>80</v>
       </c>
       <c r="E30" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="F30" s="57" t="s">
+      <c r="F30" s="56" t="s">
         <v>97</v>
       </c>
-      <c r="G30" s="57" t="s">
-        <v>134</v>
-      </c>
-      <c r="H30" s="57" t="s">
-        <v>243</v>
-      </c>
-      <c r="I30" s="57" t="s">
+      <c r="G30" s="56" t="s">
+        <v>133</v>
+      </c>
+      <c r="H30" s="56" t="s">
+        <v>242</v>
+      </c>
+      <c r="I30" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="J30" s="57" t="s">
+      <c r="J30" s="56" t="s">
         <v>69</v>
       </c>
-      <c r="K30" s="57" t="s">
-        <v>142</v>
-      </c>
-      <c r="L30" s="62"/>
-    </row>
-    <row r="31" spans="1:13" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="78" t="s">
+      <c r="K30" s="56" t="s">
+        <v>141</v>
+      </c>
+      <c r="L30" s="61"/>
+    </row>
+    <row r="31" spans="1:13" s="57" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="77" t="s">
+        <v>207</v>
+      </c>
+      <c r="B31" s="78" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="79"/>
+      <c r="D31" s="82" t="s">
+        <v>81</v>
+      </c>
+      <c r="E31" s="78" t="s">
+        <v>92</v>
+      </c>
+      <c r="F31" s="78" t="s">
+        <v>97</v>
+      </c>
+      <c r="G31" s="78" t="s">
+        <v>133</v>
+      </c>
+      <c r="H31" s="56" t="s">
+        <v>242</v>
+      </c>
+      <c r="I31" s="78" t="s">
+        <v>46</v>
+      </c>
+      <c r="J31" s="78" t="s">
+        <v>69</v>
+      </c>
+      <c r="K31" s="78" t="s">
+        <v>138</v>
+      </c>
+      <c r="L31" s="81"/>
+      <c r="M31" s="79"/>
+    </row>
+    <row r="32" spans="1:13" s="57" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="55" t="s">
         <v>208</v>
-      </c>
-      <c r="B31" s="79" t="s">
-        <v>13</v>
-      </c>
-      <c r="C31" s="80"/>
-      <c r="D31" s="83" t="s">
-        <v>81</v>
-      </c>
-      <c r="E31" s="79" t="s">
-        <v>92</v>
-      </c>
-      <c r="F31" s="79" t="s">
-        <v>97</v>
-      </c>
-      <c r="G31" s="79" t="s">
-        <v>134</v>
-      </c>
-      <c r="H31" s="57" t="s">
-        <v>243</v>
-      </c>
-      <c r="I31" s="79" t="s">
-        <v>46</v>
-      </c>
-      <c r="J31" s="79" t="s">
-        <v>69</v>
-      </c>
-      <c r="K31" s="79" t="s">
-        <v>139</v>
-      </c>
-      <c r="L31" s="82"/>
-      <c r="M31" s="80"/>
-    </row>
-    <row r="32" spans="1:13" s="58" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="56" t="s">
-        <v>209</v>
       </c>
       <c r="B32" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="C32" s="57" t="s">
+      <c r="C32" s="56" t="s">
         <v>115</v>
       </c>
-      <c r="D32" s="59" t="s">
+      <c r="D32" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="E32" s="57" t="s">
-        <v>92</v>
-      </c>
-      <c r="F32" s="57" t="s">
+      <c r="E32" s="56" t="s">
+        <v>92</v>
+      </c>
+      <c r="F32" s="56" t="s">
         <v>88</v>
       </c>
-      <c r="G32" s="57" t="s">
-        <v>134</v>
-      </c>
-      <c r="H32" s="57" t="s">
-        <v>244</v>
-      </c>
-      <c r="I32" s="57" t="s">
+      <c r="G32" s="56" t="s">
+        <v>133</v>
+      </c>
+      <c r="H32" s="56" t="s">
+        <v>243</v>
+      </c>
+      <c r="I32" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="J32" s="57" t="s">
+      <c r="J32" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="K32" s="57"/>
-      <c r="L32" s="62" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" s="58" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="56" t="s">
-        <v>210</v>
+      <c r="K32" s="56"/>
+      <c r="L32" s="61" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="55" t="s">
+        <v>209</v>
       </c>
       <c r="B33" s="34" t="s">
         <v>13</v>
       </c>
       <c r="C33" s="34" t="s">
-        <v>252</v>
-      </c>
-      <c r="D33" s="59" t="s">
-        <v>267</v>
-      </c>
-      <c r="E33" s="57" t="s">
+        <v>251</v>
+      </c>
+      <c r="D33" s="58" t="s">
+        <v>266</v>
+      </c>
+      <c r="E33" s="56" t="s">
         <v>92</v>
       </c>
       <c r="F33" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="G33" s="57" t="s">
-        <v>134</v>
-      </c>
-      <c r="H33" s="57" t="s">
-        <v>244</v>
+      <c r="G33" s="56" t="s">
+        <v>133</v>
+      </c>
+      <c r="H33" s="56" t="s">
+        <v>243</v>
       </c>
       <c r="I33" s="34" t="s">
         <v>46</v>
@@ -3199,35 +3202,35 @@
       <c r="J33" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="K33" s="57"/>
-      <c r="L33" s="62" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" s="58" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="56" t="s">
-        <v>211</v>
+      <c r="K33" s="56"/>
+      <c r="L33" s="61" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" s="57" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="55" t="s">
+        <v>210</v>
       </c>
       <c r="B34" s="34" t="s">
         <v>13</v>
       </c>
       <c r="C34" s="34" t="s">
-        <v>252</v>
-      </c>
-      <c r="D34" s="59" t="s">
-        <v>234</v>
-      </c>
-      <c r="E34" s="57" t="s">
+        <v>249</v>
+      </c>
+      <c r="D34" s="58" t="s">
+        <v>233</v>
+      </c>
+      <c r="E34" s="56" t="s">
         <v>92</v>
       </c>
       <c r="F34" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="G34" s="57" t="s">
-        <v>134</v>
-      </c>
-      <c r="H34" s="57" t="s">
-        <v>244</v>
+      <c r="G34" s="56" t="s">
+        <v>133</v>
+      </c>
+      <c r="H34" s="56" t="s">
+        <v>243</v>
       </c>
       <c r="I34" s="34" t="s">
         <v>46</v>
@@ -3235,65 +3238,65 @@
       <c r="J34" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="K34" s="57"/>
-      <c r="L34" s="62" t="s">
+      <c r="K34" s="56"/>
+      <c r="L34" s="61" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" s="79" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="77" t="s">
+        <v>211</v>
+      </c>
+      <c r="B35" s="78" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" s="34" t="s">
+        <v>249</v>
+      </c>
+      <c r="D35" s="82" t="s">
+        <v>238</v>
+      </c>
+      <c r="E35" s="78" t="s">
+        <v>92</v>
+      </c>
+      <c r="F35" s="78" t="s">
+        <v>246</v>
+      </c>
+      <c r="G35" s="78" t="s">
+        <v>133</v>
+      </c>
+      <c r="H35" s="78" t="s">
+        <v>243</v>
+      </c>
+      <c r="I35" s="86" t="s">
+        <v>89</v>
+      </c>
+      <c r="J35" s="78" t="s">
+        <v>4</v>
+      </c>
+      <c r="K35" s="78"/>
+      <c r="L35" s="81" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="35" spans="1:12" s="80" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="78" t="s">
+    <row r="36" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="49" t="s">
         <v>212</v>
-      </c>
-      <c r="B35" s="79" t="s">
-        <v>13</v>
-      </c>
-      <c r="C35" s="79" t="s">
-        <v>252</v>
-      </c>
-      <c r="D35" s="83" t="s">
-        <v>239</v>
-      </c>
-      <c r="E35" s="79" t="s">
-        <v>92</v>
-      </c>
-      <c r="F35" s="79" t="s">
-        <v>247</v>
-      </c>
-      <c r="G35" s="79" t="s">
-        <v>134</v>
-      </c>
-      <c r="H35" s="79" t="s">
-        <v>244</v>
-      </c>
-      <c r="I35" s="87" t="s">
-        <v>89</v>
-      </c>
-      <c r="J35" s="79" t="s">
-        <v>4</v>
-      </c>
-      <c r="K35" s="79"/>
-      <c r="L35" s="82" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="50" t="s">
-        <v>213</v>
       </c>
       <c r="B36" s="34" t="s">
         <v>13</v>
       </c>
       <c r="C36" s="34" t="s">
-        <v>115</v>
+        <v>326</v>
       </c>
       <c r="D36" s="30" t="s">
         <v>49</v>
       </c>
       <c r="E36" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F36" s="34" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G36" s="34">
         <v>0</v>
@@ -3309,12 +3312,12 @@
       </c>
       <c r="K36" s="34"/>
       <c r="L36" s="34" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37" s="50" t="s">
-        <v>214</v>
+      <c r="A37" s="49" t="s">
+        <v>213</v>
       </c>
       <c r="B37" s="34" t="s">
         <v>13</v>
@@ -3326,10 +3329,10 @@
         <v>75</v>
       </c>
       <c r="E37" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F37" s="34" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G37" s="34">
         <v>0</v>
@@ -3345,12 +3348,12 @@
       </c>
       <c r="K37" s="34"/>
       <c r="L37" s="34" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A38" s="50" t="s">
-        <v>215</v>
+      <c r="A38" s="49" t="s">
+        <v>214</v>
       </c>
       <c r="B38" s="36" t="s">
         <v>103</v>
@@ -3362,10 +3365,10 @@
         <v>111</v>
       </c>
       <c r="E38" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="F38" s="36" t="s">
         <v>226</v>
-      </c>
-      <c r="F38" s="36" t="s">
-        <v>227</v>
       </c>
       <c r="G38" s="34">
         <v>0</v>
@@ -3383,12 +3386,12 @@
         <v>0</v>
       </c>
       <c r="L38" s="34" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A39" s="50" t="s">
-        <v>216</v>
+      <c r="A39" s="49" t="s">
+        <v>215</v>
       </c>
       <c r="B39" s="36" t="s">
         <v>103</v>
@@ -3400,10 +3403,10 @@
         <v>44</v>
       </c>
       <c r="E39" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="F39" s="36" t="s">
         <v>226</v>
-      </c>
-      <c r="F39" s="36" t="s">
-        <v>227</v>
       </c>
       <c r="G39" s="34">
         <v>0</v>
@@ -3419,12 +3422,12 @@
       </c>
       <c r="K39" s="34"/>
       <c r="L39" s="34" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A40" s="50" t="s">
-        <v>217</v>
+      <c r="A40" s="49" t="s">
+        <v>216</v>
       </c>
       <c r="B40" s="34" t="s">
         <v>13</v>
@@ -3434,10 +3437,10 @@
         <v>114</v>
       </c>
       <c r="E40" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F40" s="34" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G40" s="34">
         <v>0</v>
@@ -3452,13 +3455,13 @@
         <v>69</v>
       </c>
       <c r="K40" s="34" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L40" s="34"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A41" s="50" t="s">
-        <v>218</v>
+      <c r="A41" s="49" t="s">
+        <v>217</v>
       </c>
       <c r="B41" s="35" t="s">
         <v>13</v>
@@ -3468,10 +3471,10 @@
         <v>43</v>
       </c>
       <c r="E41" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F41" s="34" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G41" s="35">
         <v>0</v>
@@ -3486,13 +3489,13 @@
         <v>69</v>
       </c>
       <c r="K41" s="35" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L41" s="35"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A42" s="50" t="s">
-        <v>219</v>
+      <c r="A42" s="49" t="s">
+        <v>218</v>
       </c>
       <c r="B42" s="34" t="s">
         <v>13</v>
@@ -3504,10 +3507,10 @@
         <v>50</v>
       </c>
       <c r="E42" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F42" s="34" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G42" s="34">
         <v>0</v>
@@ -3525,12 +3528,12 @@
         <v>0</v>
       </c>
       <c r="L42" s="34" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A43" s="50" t="s">
-        <v>220</v>
+      <c r="A43" s="49" t="s">
+        <v>219</v>
       </c>
       <c r="B43" s="34" t="s">
         <v>13</v>
@@ -3539,13 +3542,13 @@
         <v>113</v>
       </c>
       <c r="D43" s="30" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E43" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F43" s="34" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G43" s="34">
         <v>0</v>
@@ -3561,12 +3564,12 @@
       </c>
       <c r="K43" s="34"/>
       <c r="L43" s="34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A44" s="50" t="s">
-        <v>221</v>
+      <c r="A44" s="49" t="s">
+        <v>220</v>
       </c>
       <c r="B44" s="36" t="s">
         <v>103</v>
@@ -3576,10 +3579,10 @@
         <v>112</v>
       </c>
       <c r="E44" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F44" s="36" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G44" s="34">
         <v>0</v>
@@ -3594,13 +3597,13 @@
         <v>69</v>
       </c>
       <c r="K44" s="34" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="L44" s="34"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A45" s="50" t="s">
-        <v>222</v>
+      <c r="A45" s="49" t="s">
+        <v>221</v>
       </c>
       <c r="B45" s="36" t="s">
         <v>103</v>
@@ -3610,10 +3613,10 @@
         <v>17</v>
       </c>
       <c r="E45" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F45" s="36" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G45" s="34">
         <v>0</v>
@@ -3628,28 +3631,28 @@
         <v>69</v>
       </c>
       <c r="K45" s="34" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="L45" s="34"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A46" s="50" t="s">
-        <v>223</v>
+      <c r="A46" s="49" t="s">
+        <v>222</v>
       </c>
       <c r="B46" s="34" t="s">
         <v>13</v>
       </c>
       <c r="C46" s="34" t="s">
-        <v>115</v>
+        <v>326</v>
       </c>
       <c r="D46" s="28" t="s">
         <v>47</v>
       </c>
       <c r="E46" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F46" s="34" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G46" s="34">
         <v>0</v>
@@ -3658,34 +3661,34 @@
         <v>0</v>
       </c>
       <c r="I46" s="28" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J46" s="34" t="s">
         <v>6</v>
       </c>
       <c r="K46" s="34"/>
       <c r="L46" s="34" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A47" s="50" t="s">
-        <v>224</v>
+      <c r="A47" s="49" t="s">
+        <v>223</v>
       </c>
       <c r="B47" s="36" t="s">
         <v>103</v>
       </c>
       <c r="C47" s="36" t="s">
-        <v>116</v>
+        <v>249</v>
       </c>
       <c r="D47" s="33" t="s">
         <v>107</v>
       </c>
       <c r="E47" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F47" s="36" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="G47" s="34">
         <v>0</v>
@@ -3694,19 +3697,19 @@
         <v>0</v>
       </c>
       <c r="I47" s="28" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J47" s="34" t="s">
         <v>6</v>
       </c>
       <c r="K47" s="34"/>
       <c r="L47" s="34" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A48" s="50" t="s">
-        <v>277</v>
+      <c r="A48" s="49" t="s">
+        <v>276</v>
       </c>
       <c r="B48" s="34" t="s">
         <v>13</v>
@@ -3718,10 +3721,10 @@
         <v>108</v>
       </c>
       <c r="E48" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F48" s="34" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G48" s="34">
         <v>0</v>
@@ -3730,19 +3733,19 @@
         <v>0</v>
       </c>
       <c r="I48" s="28" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J48" s="34" t="s">
         <v>7</v>
       </c>
       <c r="K48" s="34"/>
       <c r="L48" s="34" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A49" s="50" t="s">
-        <v>278</v>
+      <c r="A49" s="49" t="s">
+        <v>277</v>
       </c>
       <c r="B49" s="34" t="s">
         <v>13</v>
@@ -3754,10 +3757,10 @@
         <v>48</v>
       </c>
       <c r="E49" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F49" s="34" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G49" s="34">
         <v>0</v>
@@ -3773,12 +3776,12 @@
       </c>
       <c r="K49" s="34"/>
       <c r="L49" s="34" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A50" s="50" t="s">
-        <v>279</v>
+      <c r="A50" s="49" t="s">
+        <v>278</v>
       </c>
       <c r="B50" s="35" t="s">
         <v>13</v>
@@ -3790,10 +3793,10 @@
         <v>48</v>
       </c>
       <c r="E50" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F50" s="34" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G50" s="35">
         <v>0</v>
@@ -3809,27 +3812,27 @@
       </c>
       <c r="K50" s="35"/>
       <c r="L50" s="35" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A51" s="50" t="s">
-        <v>280</v>
+      <c r="A51" s="49" t="s">
+        <v>279</v>
       </c>
       <c r="B51" s="34" t="s">
         <v>13</v>
       </c>
       <c r="C51" s="34" t="s">
-        <v>116</v>
+        <v>249</v>
       </c>
       <c r="D51" s="34" t="s">
         <v>67</v>
       </c>
       <c r="E51" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F51" s="34" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G51" s="34">
         <v>0</v>
@@ -3847,12 +3850,12 @@
         <v>100</v>
       </c>
       <c r="L51" s="34" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A52" s="50" t="s">
-        <v>281</v>
+      <c r="A52" s="49" t="s">
+        <v>280</v>
       </c>
       <c r="B52" s="34" t="s">
         <v>13</v>
@@ -3862,10 +3865,10 @@
         <v>66</v>
       </c>
       <c r="E52" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F52" s="34" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G52" s="34">
         <v>0</v>
@@ -3880,29 +3883,29 @@
         <v>96</v>
       </c>
       <c r="K52" s="34" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L52" s="34"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A53" s="50" t="s">
-        <v>282</v>
+      <c r="A53" s="49" t="s">
+        <v>281</v>
       </c>
       <c r="B53" s="34" t="s">
         <v>13</v>
       </c>
       <c r="C53" s="34"/>
       <c r="D53" s="30" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E53" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F53" s="34" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G53" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H53" s="34">
         <v>0</v>
@@ -3914,13 +3917,13 @@
         <v>69</v>
       </c>
       <c r="K53" s="34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="L53" s="34"/>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A54" s="50" t="s">
-        <v>283</v>
+      <c r="A54" s="49" t="s">
+        <v>282</v>
       </c>
       <c r="B54" s="34" t="s">
         <v>13</v>
@@ -3930,10 +3933,10 @@
         <v>74</v>
       </c>
       <c r="E54" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F54" s="34" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G54" s="34">
         <v>0</v>
@@ -3948,13 +3951,13 @@
         <v>69</v>
       </c>
       <c r="K54" s="34" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L54" s="34"/>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A55" s="50" t="s">
-        <v>284</v>
+      <c r="A55" s="49" t="s">
+        <v>283</v>
       </c>
       <c r="B55" s="34" t="s">
         <v>13</v>
@@ -3966,31 +3969,31 @@
         <v>109</v>
       </c>
       <c r="E55" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F55" s="34" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G55" s="34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H55" s="34">
         <v>0</v>
       </c>
       <c r="I55" s="28" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J55" s="34" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K55" s="34"/>
       <c r="L55" s="34" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A56" s="50" t="s">
-        <v>285</v>
+      <c r="A56" s="49" t="s">
+        <v>284</v>
       </c>
       <c r="B56" s="34" t="s">
         <v>13</v>
@@ -4002,10 +4005,10 @@
         <v>87</v>
       </c>
       <c r="E56" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F56" s="34" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G56" s="34">
         <v>0</v>
@@ -4020,172 +4023,172 @@
         <v>69</v>
       </c>
       <c r="K56" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="L56" s="34"/>
+    </row>
+    <row r="57" spans="1:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="49" t="s">
+        <v>285</v>
+      </c>
+      <c r="B57" s="78" t="s">
+        <v>13</v>
+      </c>
+      <c r="C57" s="79"/>
+      <c r="D57" s="87" t="s">
+        <v>197</v>
+      </c>
+      <c r="E57" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="F57" s="78" t="s">
+        <v>229</v>
+      </c>
+      <c r="G57" s="78">
+        <v>0</v>
+      </c>
+      <c r="H57" s="78">
+        <v>0</v>
+      </c>
+      <c r="I57" s="87" t="s">
+        <v>90</v>
+      </c>
+      <c r="J57" s="78" t="s">
+        <v>69</v>
+      </c>
+      <c r="K57" s="78" t="s">
         <v>140</v>
       </c>
-      <c r="L56" s="34"/>
-    </row>
-    <row r="57" spans="1:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="50" t="s">
+      <c r="L57" s="81"/>
+    </row>
+    <row r="58" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="49" t="s">
         <v>286</v>
-      </c>
-      <c r="B57" s="79" t="s">
-        <v>13</v>
-      </c>
-      <c r="C57" s="80"/>
-      <c r="D57" s="88" t="s">
-        <v>198</v>
-      </c>
-      <c r="E57" s="79" t="s">
-        <v>226</v>
-      </c>
-      <c r="F57" s="79" t="s">
-        <v>230</v>
-      </c>
-      <c r="G57" s="79">
-        <v>0</v>
-      </c>
-      <c r="H57" s="79">
-        <v>0</v>
-      </c>
-      <c r="I57" s="88" t="s">
-        <v>90</v>
-      </c>
-      <c r="J57" s="79" t="s">
-        <v>69</v>
-      </c>
-      <c r="K57" s="79" t="s">
-        <v>141</v>
-      </c>
-      <c r="L57" s="82"/>
-    </row>
-    <row r="58" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="50" t="s">
-        <v>287</v>
       </c>
       <c r="B58" s="34" t="s">
         <v>13</v>
       </c>
       <c r="C58" s="34" t="s">
-        <v>250</v>
-      </c>
-      <c r="D58" s="90" t="s">
-        <v>245</v>
+        <v>249</v>
+      </c>
+      <c r="D58" s="89" t="s">
+        <v>244</v>
       </c>
       <c r="E58" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F58" s="34" t="s">
-        <v>225</v>
-      </c>
-      <c r="G58" s="57" t="s">
-        <v>134</v>
-      </c>
-      <c r="H58" s="57" t="s">
-        <v>243</v>
+        <v>224</v>
+      </c>
+      <c r="G58" s="56" t="s">
+        <v>133</v>
+      </c>
+      <c r="H58" s="56" t="s">
+        <v>242</v>
       </c>
       <c r="I58" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="J58" s="57" t="s">
+      <c r="J58" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="K58" s="57"/>
-      <c r="L58" s="62" t="s">
-        <v>249</v>
+      <c r="K58" s="56"/>
+      <c r="L58" s="61" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A59" s="50" t="s">
-        <v>288</v>
+      <c r="A59" s="49" t="s">
+        <v>287</v>
       </c>
       <c r="B59" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="C59" s="58"/>
-      <c r="D59" s="59" t="s">
+      <c r="C59" s="57"/>
+      <c r="D59" s="58" t="s">
         <v>80</v>
       </c>
       <c r="E59" s="34" t="s">
-        <v>226</v>
-      </c>
-      <c r="F59" s="57" t="s">
         <v>225</v>
       </c>
-      <c r="G59" s="57" t="s">
-        <v>134</v>
-      </c>
-      <c r="H59" s="57" t="s">
-        <v>243</v>
-      </c>
-      <c r="I59" s="57" t="s">
+      <c r="F59" s="56" t="s">
+        <v>224</v>
+      </c>
+      <c r="G59" s="56" t="s">
+        <v>133</v>
+      </c>
+      <c r="H59" s="56" t="s">
+        <v>242</v>
+      </c>
+      <c r="I59" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="J59" s="57" t="s">
+      <c r="J59" s="56" t="s">
         <v>69</v>
       </c>
-      <c r="K59" s="57" t="s">
-        <v>142</v>
-      </c>
-      <c r="L59" s="62"/>
+      <c r="K59" s="56" t="s">
+        <v>141</v>
+      </c>
+      <c r="L59" s="61"/>
     </row>
     <row r="60" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="50" t="s">
+      <c r="A60" s="49" t="s">
+        <v>288</v>
+      </c>
+      <c r="B60" s="78" t="s">
+        <v>13</v>
+      </c>
+      <c r="C60" s="79"/>
+      <c r="D60" s="82" t="s">
+        <v>81</v>
+      </c>
+      <c r="E60" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="F60" s="56" t="s">
+        <v>224</v>
+      </c>
+      <c r="G60" s="78" t="s">
+        <v>133</v>
+      </c>
+      <c r="H60" s="56" t="s">
+        <v>242</v>
+      </c>
+      <c r="I60" s="78" t="s">
+        <v>46</v>
+      </c>
+      <c r="J60" s="78" t="s">
+        <v>69</v>
+      </c>
+      <c r="K60" s="78" t="s">
+        <v>138</v>
+      </c>
+      <c r="L60" s="81"/>
+    </row>
+    <row r="61" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="49" t="s">
         <v>289</v>
-      </c>
-      <c r="B60" s="79" t="s">
-        <v>13</v>
-      </c>
-      <c r="C60" s="80"/>
-      <c r="D60" s="83" t="s">
-        <v>81</v>
-      </c>
-      <c r="E60" s="79" t="s">
-        <v>226</v>
-      </c>
-      <c r="F60" s="57" t="s">
-        <v>225</v>
-      </c>
-      <c r="G60" s="79" t="s">
-        <v>134</v>
-      </c>
-      <c r="H60" s="57" t="s">
-        <v>243</v>
-      </c>
-      <c r="I60" s="79" t="s">
-        <v>46</v>
-      </c>
-      <c r="J60" s="79" t="s">
-        <v>69</v>
-      </c>
-      <c r="K60" s="79" t="s">
-        <v>139</v>
-      </c>
-      <c r="L60" s="82"/>
-    </row>
-    <row r="61" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="50" t="s">
-        <v>290</v>
       </c>
       <c r="B61" s="34" t="s">
         <v>13</v>
       </c>
       <c r="C61" s="34" t="s">
-        <v>252</v>
-      </c>
-      <c r="D61" s="59" t="s">
-        <v>234</v>
+        <v>249</v>
+      </c>
+      <c r="D61" s="58" t="s">
+        <v>233</v>
       </c>
       <c r="E61" s="34" t="s">
-        <v>226</v>
-      </c>
-      <c r="F61" s="57" t="s">
         <v>225</v>
       </c>
-      <c r="G61" s="57" t="s">
-        <v>134</v>
-      </c>
-      <c r="H61" s="57" t="s">
-        <v>244</v>
+      <c r="F61" s="56" t="s">
+        <v>224</v>
+      </c>
+      <c r="G61" s="56" t="s">
+        <v>133</v>
+      </c>
+      <c r="H61" s="56" t="s">
+        <v>243</v>
       </c>
       <c r="I61" s="34" t="s">
         <v>46</v>
@@ -4193,57 +4196,57 @@
       <c r="J61" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="K61" s="57"/>
-      <c r="L61" s="62" t="s">
+      <c r="K61" s="56"/>
+      <c r="L61" s="61" t="s">
+        <v>253</v>
+      </c>
+      <c r="M61" s="61" t="s">
+        <v>253</v>
+      </c>
+      <c r="N61" s="61" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="49" t="s">
+        <v>290</v>
+      </c>
+      <c r="B62" s="78" t="s">
+        <v>13</v>
+      </c>
+      <c r="C62" s="34" t="s">
+        <v>249</v>
+      </c>
+      <c r="D62" s="82" t="s">
+        <v>238</v>
+      </c>
+      <c r="E62" s="78" t="s">
+        <v>225</v>
+      </c>
+      <c r="F62" s="78" t="s">
+        <v>275</v>
+      </c>
+      <c r="G62" s="78" t="s">
+        <v>133</v>
+      </c>
+      <c r="H62" s="78" t="s">
+        <v>243</v>
+      </c>
+      <c r="I62" s="88" t="s">
+        <v>89</v>
+      </c>
+      <c r="J62" s="78" t="s">
+        <v>4</v>
+      </c>
+      <c r="K62" s="78"/>
+      <c r="L62" s="81" t="s">
         <v>254</v>
       </c>
-      <c r="M61" s="62" t="s">
+      <c r="M62" s="81" t="s">
         <v>254</v>
       </c>
-      <c r="N61" s="62" t="s">
+      <c r="N62" s="81" t="s">
         <v>254</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="50" t="s">
-        <v>291</v>
-      </c>
-      <c r="B62" s="79" t="s">
-        <v>13</v>
-      </c>
-      <c r="C62" s="79" t="s">
-        <v>252</v>
-      </c>
-      <c r="D62" s="83" t="s">
-        <v>239</v>
-      </c>
-      <c r="E62" s="79" t="s">
-        <v>226</v>
-      </c>
-      <c r="F62" s="79" t="s">
-        <v>276</v>
-      </c>
-      <c r="G62" s="79" t="s">
-        <v>134</v>
-      </c>
-      <c r="H62" s="79" t="s">
-        <v>244</v>
-      </c>
-      <c r="I62" s="89" t="s">
-        <v>89</v>
-      </c>
-      <c r="J62" s="79" t="s">
-        <v>4</v>
-      </c>
-      <c r="K62" s="79"/>
-      <c r="L62" s="82" t="s">
-        <v>255</v>
-      </c>
-      <c r="M62" s="82" t="s">
-        <v>255</v>
-      </c>
-      <c r="N62" s="82" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="63" spans="1:14" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
@@ -4257,8 +4260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H89"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4274,32 +4277,32 @@
   <sheetData>
     <row r="1" spans="1:8" s="20" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C1" s="20" t="s">
         <v>91</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E1" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" s="20" t="s">
         <v>149</v>
       </c>
-      <c r="F1" s="20" t="s">
-        <v>150</v>
-      </c>
       <c r="G1" s="20" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H1" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="101" t="s">
+      <c r="A2" s="100" t="s">
         <v>84</v>
       </c>
       <c r="B2" s="22" t="s">
@@ -4312,7 +4315,7 @@
         <v>70</v>
       </c>
       <c r="F2" s="32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G2" s="38"/>
       <c r="H2" s="38"/>
@@ -4328,7 +4331,7 @@
         <v>23</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -4342,7 +4345,7 @@
         <v>24</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -4356,7 +4359,7 @@
         <v>25</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -4370,7 +4373,7 @@
         <v>26</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -4386,7 +4389,7 @@
         <v>27</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G7" s="23"/>
       <c r="H7" s="23"/>
@@ -4395,127 +4398,127 @@
       <c r="B8" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="C8" s="54" t="s">
+      <c r="C8" s="53" t="s">
         <v>92</v>
       </c>
       <c r="E8" s="32" t="s">
         <v>71</v>
       </c>
       <c r="F8" s="32" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G8" s="38"/>
       <c r="H8" s="38" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="C9" s="54" t="s">
+      <c r="C9" s="53" t="s">
         <v>92</v>
       </c>
       <c r="E9" s="22" t="s">
         <v>28</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G9" s="22" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="103"/>
-      <c r="B10" s="103" t="s">
+      <c r="A10" s="102"/>
+      <c r="B10" s="102" t="s">
         <v>85</v>
       </c>
-      <c r="C10" s="106" t="s">
-        <v>92</v>
-      </c>
-      <c r="D10" s="103"/>
-      <c r="E10" s="103" t="s">
+      <c r="C10" s="105" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" s="102"/>
+      <c r="E10" s="102" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="103" t="s">
-        <v>163</v>
-      </c>
-      <c r="G10" s="103" t="s">
+      <c r="F10" s="102" t="s">
+        <v>162</v>
+      </c>
+      <c r="G10" s="102" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="103"/>
+      <c r="H10" s="102"/>
     </row>
     <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="54" t="s">
-        <v>92</v>
-      </c>
-      <c r="D11" s="51" t="s">
-        <v>153</v>
+      <c r="C11" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" s="50" t="s">
+        <v>152</v>
       </c>
       <c r="E11" s="32" t="s">
         <v>72</v>
       </c>
       <c r="F11" s="32" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G11" s="38"/>
       <c r="H11" s="38" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="54" t="s">
-        <v>92</v>
-      </c>
-      <c r="D12" s="51" t="s">
-        <v>153</v>
-      </c>
-      <c r="E12" s="51" t="s">
+      <c r="C12" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" s="50" t="s">
+        <v>152</v>
+      </c>
+      <c r="E12" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="51" t="s">
-        <v>164</v>
+      <c r="F12" s="50" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="54" t="s">
-        <v>92</v>
-      </c>
-      <c r="D13" s="51" t="s">
-        <v>153</v>
-      </c>
-      <c r="E13" s="51" t="s">
+      <c r="C13" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" s="50" t="s">
+        <v>152</v>
+      </c>
+      <c r="E13" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="51" t="s">
-        <v>188</v>
+      <c r="F13" s="50" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="54" t="s">
-        <v>92</v>
-      </c>
-      <c r="D14" s="51" t="s">
-        <v>153</v>
-      </c>
-      <c r="E14" s="51" t="s">
+      <c r="C14" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" s="50" t="s">
+        <v>152</v>
+      </c>
+      <c r="E14" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="F14" s="51" t="s">
-        <v>189</v>
+      <c r="F14" s="50" t="s">
+        <v>188</v>
       </c>
       <c r="G14" s="22" t="s">
         <v>35</v>
@@ -4525,17 +4528,17 @@
       <c r="B15" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="54" t="s">
-        <v>92</v>
-      </c>
-      <c r="D15" s="51" t="s">
-        <v>153</v>
-      </c>
-      <c r="E15" s="51" t="s">
+      <c r="C15" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" s="50" t="s">
+        <v>152</v>
+      </c>
+      <c r="E15" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="51" t="s">
-        <v>190</v>
+      <c r="F15" s="50" t="s">
+        <v>189</v>
       </c>
       <c r="G15" s="22" t="s">
         <v>37</v>
@@ -4545,58 +4548,58 @@
       <c r="B16" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="54" t="s">
-        <v>92</v>
-      </c>
-      <c r="D16" s="51" t="s">
-        <v>153</v>
-      </c>
-      <c r="E16" s="51" t="s">
+      <c r="C16" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="50" t="s">
+        <v>152</v>
+      </c>
+      <c r="E16" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="51" t="s">
-        <v>191</v>
+      <c r="F16" s="50" t="s">
+        <v>190</v>
       </c>
       <c r="G16" s="22" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="66.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="107" t="s">
+      <c r="B17" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="108" t="s">
-        <v>92</v>
-      </c>
-      <c r="D17" s="109" t="s">
-        <v>153</v>
-      </c>
-      <c r="E17" s="109" t="s">
+      <c r="C17" s="107" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="108" t="s">
+        <v>152</v>
+      </c>
+      <c r="E17" s="108" t="s">
         <v>40</v>
       </c>
-      <c r="F17" s="109" t="s">
-        <v>192</v>
-      </c>
-      <c r="G17" s="107" t="s">
+      <c r="F17" s="108" t="s">
+        <v>191</v>
+      </c>
+      <c r="G17" s="106" t="s">
         <v>41</v>
       </c>
-      <c r="H17" s="107"/>
+      <c r="H17" s="106"/>
     </row>
     <row r="18" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="54" t="s">
-        <v>92</v>
-      </c>
-      <c r="D18" s="52" t="s">
-        <v>154</v>
+      <c r="C18" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" s="51" t="s">
+        <v>153</v>
       </c>
       <c r="E18" s="32" t="s">
         <v>42</v>
       </c>
       <c r="F18" s="32" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G18" s="38"/>
       <c r="H18" s="38"/>
@@ -4605,68 +4608,68 @@
       <c r="B19" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="54" t="s">
-        <v>92</v>
-      </c>
-      <c r="D19" s="52" t="s">
-        <v>154</v>
-      </c>
-      <c r="E19" s="52" t="s">
+      <c r="C19" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="51" t="s">
+        <v>153</v>
+      </c>
+      <c r="E19" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="52" t="s">
-        <v>178</v>
+      <c r="F19" s="51" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="54" t="s">
-        <v>92</v>
-      </c>
-      <c r="D20" s="52" t="s">
-        <v>154</v>
-      </c>
-      <c r="E20" s="52" t="s">
+      <c r="C20" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" s="51" t="s">
+        <v>153</v>
+      </c>
+      <c r="E20" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="F20" s="52" t="s">
-        <v>177</v>
+      <c r="F20" s="51" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="54" t="s">
-        <v>92</v>
-      </c>
-      <c r="D21" s="52" t="s">
-        <v>154</v>
-      </c>
-      <c r="E21" s="52" t="s">
+      <c r="C21" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" s="51" t="s">
+        <v>153</v>
+      </c>
+      <c r="E21" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="F21" s="52" t="s">
-        <v>179</v>
+      <c r="F21" s="51" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="54" t="s">
-        <v>92</v>
-      </c>
-      <c r="D22" s="52" t="s">
-        <v>154</v>
-      </c>
-      <c r="E22" s="52" t="s">
+      <c r="C22" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="D22" s="51" t="s">
+        <v>153</v>
+      </c>
+      <c r="E22" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="F22" s="52" t="s">
-        <v>180</v>
+      <c r="F22" s="51" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -4674,36 +4677,36 @@
       <c r="B23" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="55" t="s">
-        <v>92</v>
-      </c>
-      <c r="D23" s="53" t="s">
-        <v>154</v>
-      </c>
-      <c r="E23" s="53" t="s">
+      <c r="C23" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23" s="52" t="s">
+        <v>153</v>
+      </c>
+      <c r="E23" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="53" t="s">
-        <v>181</v>
+      <c r="F23" s="52" t="s">
+        <v>180</v>
       </c>
       <c r="G23" s="23"/>
-      <c r="H23" s="103"/>
+      <c r="H23" s="102"/>
     </row>
     <row r="24" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="C24" s="54" t="s">
-        <v>92</v>
-      </c>
-      <c r="D24" s="51" t="s">
-        <v>155</v>
+      <c r="C24" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" s="50" t="s">
+        <v>154</v>
       </c>
       <c r="E24" s="32" t="s">
         <v>73</v>
       </c>
       <c r="F24" s="32" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G24" s="38"/>
       <c r="H24" s="38"/>
@@ -4712,17 +4715,17 @@
       <c r="B25" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="C25" s="54" t="s">
-        <v>92</v>
-      </c>
-      <c r="D25" s="51" t="s">
-        <v>155</v>
-      </c>
-      <c r="E25" s="51" t="s">
+      <c r="C25" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="D25" s="50" t="s">
+        <v>154</v>
+      </c>
+      <c r="E25" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="F25" s="51" t="s">
-        <v>193</v>
+      <c r="F25" s="50" t="s">
+        <v>192</v>
       </c>
       <c r="G25" s="22" t="s">
         <v>52</v>
@@ -4732,17 +4735,17 @@
       <c r="B26" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="C26" s="54" t="s">
-        <v>92</v>
-      </c>
-      <c r="D26" s="51" t="s">
-        <v>155</v>
-      </c>
-      <c r="E26" s="51" t="s">
+      <c r="C26" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="D26" s="50" t="s">
+        <v>154</v>
+      </c>
+      <c r="E26" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="F26" s="51" t="s">
-        <v>194</v>
+      <c r="F26" s="50" t="s">
+        <v>193</v>
       </c>
       <c r="G26" s="22" t="s">
         <v>54</v>
@@ -4752,75 +4755,75 @@
       <c r="B27" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="C27" s="54" t="s">
-        <v>92</v>
-      </c>
-      <c r="D27" s="51" t="s">
-        <v>155</v>
-      </c>
-      <c r="E27" s="51" t="s">
+      <c r="C27" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27" s="50" t="s">
+        <v>154</v>
+      </c>
+      <c r="E27" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="F27" s="51" t="s">
-        <v>195</v>
+      <c r="F27" s="50" t="s">
+        <v>194</v>
       </c>
       <c r="G27" s="22" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="107" t="s">
+      <c r="B28" s="106" t="s">
         <v>94</v>
       </c>
-      <c r="C28" s="108" t="s">
-        <v>92</v>
-      </c>
-      <c r="D28" s="109" t="s">
-        <v>155</v>
-      </c>
-      <c r="E28" s="109" t="s">
+      <c r="C28" s="107" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" s="108" t="s">
+        <v>154</v>
+      </c>
+      <c r="E28" s="108" t="s">
         <v>57</v>
       </c>
-      <c r="F28" s="109" t="s">
-        <v>196</v>
-      </c>
-      <c r="G28" s="107" t="s">
+      <c r="F28" s="108" t="s">
+        <v>195</v>
+      </c>
+      <c r="G28" s="106" t="s">
         <v>58</v>
       </c>
-      <c r="H28" s="107"/>
+      <c r="H28" s="106"/>
     </row>
     <row r="29" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="C29" s="54" t="s">
-        <v>92</v>
-      </c>
-      <c r="D29" s="52" t="s">
-        <v>154</v>
+      <c r="C29" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="D29" s="51" t="s">
+        <v>153</v>
       </c>
       <c r="E29" s="32" t="s">
         <v>59</v>
       </c>
       <c r="F29" s="32" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="C30" s="54" t="s">
-        <v>92</v>
-      </c>
-      <c r="D30" s="52" t="s">
-        <v>154</v>
-      </c>
-      <c r="E30" s="52" t="s">
+      <c r="C30" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="D30" s="51" t="s">
+        <v>153</v>
+      </c>
+      <c r="E30" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="F30" s="52" t="s">
-        <v>197</v>
+      <c r="F30" s="51" t="s">
+        <v>196</v>
       </c>
       <c r="G30" s="22" t="s">
         <v>61</v>
@@ -4830,46 +4833,46 @@
       <c r="B31" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="C31" s="54" t="s">
-        <v>92</v>
-      </c>
-      <c r="D31" s="52" t="s">
-        <v>154</v>
-      </c>
-      <c r="E31" s="52" t="s">
+      <c r="C31" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="D31" s="51" t="s">
+        <v>153</v>
+      </c>
+      <c r="E31" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="F31" s="52" t="s">
-        <v>200</v>
+      <c r="F31" s="51" t="s">
+        <v>199</v>
       </c>
       <c r="G31" s="22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="71"/>
-      <c r="B32" s="71" t="s">
+      <c r="A32" s="70"/>
+      <c r="B32" s="70" t="s">
         <v>94</v>
       </c>
-      <c r="C32" s="72" t="s">
-        <v>92</v>
-      </c>
-      <c r="D32" s="74" t="s">
-        <v>154</v>
-      </c>
-      <c r="E32" s="74" t="s">
+      <c r="C32" s="71" t="s">
+        <v>92</v>
+      </c>
+      <c r="D32" s="73" t="s">
+        <v>153</v>
+      </c>
+      <c r="E32" s="73" t="s">
         <v>64</v>
       </c>
-      <c r="F32" s="74" t="s">
-        <v>175</v>
-      </c>
-      <c r="G32" s="71" t="s">
+      <c r="F32" s="73" t="s">
+        <v>174</v>
+      </c>
+      <c r="G32" s="70" t="s">
         <v>65</v>
       </c>
-      <c r="H32" s="71"/>
+      <c r="H32" s="70"/>
     </row>
     <row r="33" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="102" t="s">
+      <c r="A33" s="101" t="s">
         <v>95</v>
       </c>
       <c r="B33" s="22" t="s">
@@ -4879,302 +4882,302 @@
         <v>70</v>
       </c>
       <c r="F33" s="38" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B34" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E34" s="67" t="s">
+      <c r="E34" s="66" t="s">
         <v>76</v>
       </c>
       <c r="F34" s="22" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B35" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E35" s="67" t="s">
+      <c r="E35" s="66" t="s">
         <v>77</v>
       </c>
       <c r="F35" s="22" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B36" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E36" s="67" t="s">
+      <c r="E36" s="66" t="s">
         <v>78</v>
       </c>
       <c r="F36" s="22" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B37" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="C37" s="105" t="s">
-        <v>92</v>
-      </c>
-      <c r="E37" s="70" t="s">
+      <c r="C37" s="104" t="s">
+        <v>92</v>
+      </c>
+      <c r="E37" s="69" t="s">
         <v>71</v>
       </c>
       <c r="F37" s="38" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B38" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="C38" s="105" t="s">
-        <v>92</v>
-      </c>
-      <c r="D38" s="52" t="s">
-        <v>154</v>
-      </c>
-      <c r="E38" s="69" t="s">
+      <c r="C38" s="104" t="s">
+        <v>92</v>
+      </c>
+      <c r="D38" s="51" t="s">
+        <v>153</v>
+      </c>
+      <c r="E38" s="68" t="s">
         <v>79</v>
       </c>
-      <c r="F38" s="52" t="s">
-        <v>261</v>
+      <c r="F38" s="51" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B39" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="C39" s="105" t="s">
-        <v>92</v>
-      </c>
-      <c r="E39" s="67" t="s">
+      <c r="C39" s="104" t="s">
+        <v>92</v>
+      </c>
+      <c r="E39" s="66" t="s">
         <v>80</v>
       </c>
       <c r="F39" s="22" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="70"/>
+      <c r="B40" s="70" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40" s="71" t="s">
+        <v>92</v>
+      </c>
+      <c r="D40" s="70"/>
+      <c r="E40" s="72" t="s">
+        <v>81</v>
+      </c>
+      <c r="F40" s="70" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="71"/>
-      <c r="B40" s="71" t="s">
-        <v>85</v>
-      </c>
-      <c r="C40" s="72" t="s">
-        <v>92</v>
-      </c>
-      <c r="D40" s="71"/>
-      <c r="E40" s="73" t="s">
-        <v>81</v>
-      </c>
-      <c r="F40" s="71" t="s">
-        <v>263</v>
-      </c>
-      <c r="G40" s="71"/>
-      <c r="H40" s="71"/>
+      <c r="G40" s="70"/>
+      <c r="H40" s="70"/>
     </row>
     <row r="41" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="102" t="s">
-        <v>231</v>
+      <c r="A41" s="101" t="s">
+        <v>230</v>
       </c>
       <c r="B41" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E41" s="75" t="s">
+      <c r="E41" s="74" t="s">
         <v>70</v>
       </c>
-      <c r="F41" s="84" t="s">
-        <v>269</v>
-      </c>
-      <c r="G41" s="93"/>
-      <c r="H41" s="93"/>
+      <c r="F41" s="83" t="s">
+        <v>268</v>
+      </c>
+      <c r="G41" s="92"/>
+      <c r="H41" s="92"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B42" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E42" s="64" t="s">
+      <c r="E42" s="63" t="s">
         <v>76</v>
       </c>
       <c r="F42" s="22" t="s">
-        <v>265</v>
-      </c>
-      <c r="G42" s="66"/>
-      <c r="H42" s="93"/>
+        <v>264</v>
+      </c>
+      <c r="G42" s="65"/>
+      <c r="H42" s="92"/>
     </row>
     <row r="43" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B43" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E43" s="64" t="s">
-        <v>232</v>
+      <c r="E43" s="63" t="s">
+        <v>231</v>
       </c>
       <c r="F43" s="22" t="s">
-        <v>266</v>
-      </c>
-      <c r="G43" s="93"/>
-      <c r="H43" s="93"/>
+        <v>265</v>
+      </c>
+      <c r="G43" s="92"/>
+      <c r="H43" s="92"/>
     </row>
     <row r="44" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B44" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E44" s="64" t="s">
-        <v>233</v>
+      <c r="E44" s="63" t="s">
+        <v>232</v>
       </c>
       <c r="F44" s="22" t="s">
-        <v>268</v>
-      </c>
-      <c r="G44" s="66"/>
-      <c r="H44" s="93"/>
+        <v>267</v>
+      </c>
+      <c r="G44" s="65"/>
+      <c r="H44" s="92"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B45" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="C45" s="55" t="s">
-        <v>92</v>
-      </c>
-      <c r="E45" s="76" t="s">
+      <c r="C45" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="E45" s="75" t="s">
         <v>71</v>
       </c>
       <c r="F45" s="38" t="s">
-        <v>273</v>
-      </c>
-      <c r="G45" s="66"/>
-      <c r="H45" s="93"/>
+        <v>272</v>
+      </c>
+      <c r="G45" s="65"/>
+      <c r="H45" s="92"/>
     </row>
     <row r="46" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B46" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="C46" s="55" t="s">
-        <v>92</v>
-      </c>
-      <c r="E46" s="64" t="s">
-        <v>234</v>
+      <c r="C46" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="E46" s="63" t="s">
+        <v>233</v>
       </c>
       <c r="F46" s="22" t="s">
-        <v>270</v>
-      </c>
-      <c r="G46" s="66"/>
-      <c r="H46" s="93"/>
+        <v>269</v>
+      </c>
+      <c r="G46" s="65"/>
+      <c r="H46" s="92"/>
     </row>
     <row r="47" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B47" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="C47" s="55" t="s">
-        <v>92</v>
-      </c>
-      <c r="E47" s="64" t="s">
-        <v>235</v>
+      <c r="C47" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="E47" s="63" t="s">
+        <v>234</v>
       </c>
       <c r="F47" s="22" t="s">
-        <v>271</v>
-      </c>
-      <c r="G47" s="66"/>
-      <c r="H47" s="93"/>
+        <v>270</v>
+      </c>
+      <c r="G47" s="65"/>
+      <c r="H47" s="92"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B48" s="22" t="s">
+        <v>235</v>
+      </c>
+      <c r="C48" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="D48" s="50" t="s">
+        <v>154</v>
+      </c>
+      <c r="E48" s="75" t="s">
         <v>236</v>
       </c>
-      <c r="C48" s="55" t="s">
-        <v>92</v>
-      </c>
-      <c r="D48" s="51" t="s">
-        <v>155</v>
-      </c>
-      <c r="E48" s="76" t="s">
-        <v>237</v>
-      </c>
       <c r="F48" s="38" t="s">
-        <v>274</v>
-      </c>
-      <c r="G48" s="66"/>
-      <c r="H48" s="93"/>
+        <v>273</v>
+      </c>
+      <c r="G48" s="65"/>
+      <c r="H48" s="92"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B49" s="22" t="s">
-        <v>236</v>
-      </c>
-      <c r="C49" s="55" t="s">
-        <v>92</v>
-      </c>
-      <c r="D49" s="51" t="s">
-        <v>155</v>
-      </c>
-      <c r="E49" s="85" t="s">
+        <v>235</v>
+      </c>
+      <c r="C49" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="D49" s="50" t="s">
+        <v>154</v>
+      </c>
+      <c r="E49" s="84" t="s">
+        <v>237</v>
+      </c>
+      <c r="F49" s="50" t="s">
+        <v>274</v>
+      </c>
+      <c r="G49" s="63" t="s">
         <v>238</v>
       </c>
-      <c r="F49" s="51" t="s">
-        <v>275</v>
-      </c>
-      <c r="G49" s="64" t="s">
+    </row>
+    <row r="50" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="70"/>
+      <c r="B50" s="70" t="s">
+        <v>235</v>
+      </c>
+      <c r="C50" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="D50" s="50" t="s">
+        <v>154</v>
+      </c>
+      <c r="E50" s="85" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="71"/>
-      <c r="B50" s="71" t="s">
-        <v>236</v>
-      </c>
-      <c r="C50" s="55" t="s">
-        <v>92</v>
-      </c>
-      <c r="D50" s="51" t="s">
-        <v>155</v>
-      </c>
-      <c r="E50" s="86" t="s">
+      <c r="F50" s="50" t="s">
+        <v>271</v>
+      </c>
+      <c r="G50" s="76" t="s">
         <v>240</v>
       </c>
-      <c r="F50" s="51" t="s">
-        <v>272</v>
-      </c>
-      <c r="G50" s="77" t="s">
-        <v>241</v>
-      </c>
-      <c r="H50" s="71"/>
+      <c r="H50" s="70"/>
     </row>
     <row r="51" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="101" t="s">
+      <c r="A51" s="100" t="s">
         <v>84</v>
       </c>
       <c r="B51" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="C51" s="91" t="s">
-        <v>226</v>
+      <c r="C51" s="90" t="s">
+        <v>225</v>
       </c>
       <c r="E51" s="38" t="s">
         <v>71</v>
       </c>
       <c r="F51" s="38" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G51" s="38"/>
       <c r="H51" s="38" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B52" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="C52" s="91" t="s">
-        <v>226</v>
+      <c r="C52" s="90" t="s">
+        <v>225</v>
       </c>
       <c r="E52" s="22" t="s">
         <v>28</v>
       </c>
       <c r="F52" s="22" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G52" s="22" t="s">
         <v>29</v>
@@ -5184,14 +5187,14 @@
       <c r="B53" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="C53" s="91" t="s">
-        <v>226</v>
+      <c r="C53" s="90" t="s">
+        <v>225</v>
       </c>
       <c r="E53" s="22" t="s">
         <v>30</v>
       </c>
       <c r="F53" s="22" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G53" s="22" t="s">
         <v>31</v>
@@ -5201,72 +5204,72 @@
       <c r="B54" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C54" s="91" t="s">
-        <v>226</v>
-      </c>
-      <c r="D54" s="94" t="s">
-        <v>153</v>
+      <c r="C54" s="90" t="s">
+        <v>225</v>
+      </c>
+      <c r="D54" s="93" t="s">
+        <v>152</v>
       </c>
       <c r="E54" s="38" t="s">
         <v>72</v>
       </c>
       <c r="F54" s="38" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G54" s="38"/>
       <c r="H54" s="38" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B55" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C55" s="91" t="s">
-        <v>226</v>
-      </c>
-      <c r="D55" s="94" t="s">
-        <v>153</v>
-      </c>
-      <c r="E55" s="94" t="s">
+      <c r="C55" s="90" t="s">
+        <v>225</v>
+      </c>
+      <c r="D55" s="93" t="s">
+        <v>152</v>
+      </c>
+      <c r="E55" s="93" t="s">
         <v>32</v>
       </c>
-      <c r="F55" s="94" t="s">
-        <v>296</v>
+      <c r="F55" s="93" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B56" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C56" s="91" t="s">
-        <v>226</v>
-      </c>
-      <c r="D56" s="94" t="s">
-        <v>153</v>
-      </c>
-      <c r="E56" s="94" t="s">
+      <c r="C56" s="90" t="s">
+        <v>225</v>
+      </c>
+      <c r="D56" s="93" t="s">
+        <v>152</v>
+      </c>
+      <c r="E56" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="F56" s="94" t="s">
-        <v>297</v>
+      <c r="F56" s="93" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B57" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C57" s="91" t="s">
-        <v>226</v>
-      </c>
-      <c r="D57" s="94" t="s">
-        <v>153</v>
-      </c>
-      <c r="E57" s="94" t="s">
+      <c r="C57" s="90" t="s">
+        <v>225</v>
+      </c>
+      <c r="D57" s="93" t="s">
+        <v>152</v>
+      </c>
+      <c r="E57" s="93" t="s">
         <v>34</v>
       </c>
-      <c r="F57" s="94" t="s">
-        <v>298</v>
+      <c r="F57" s="93" t="s">
+        <v>297</v>
       </c>
       <c r="G57" s="22" t="s">
         <v>35</v>
@@ -5276,17 +5279,17 @@
       <c r="B58" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C58" s="91" t="s">
-        <v>226</v>
-      </c>
-      <c r="D58" s="94" t="s">
-        <v>153</v>
-      </c>
-      <c r="E58" s="94" t="s">
+      <c r="C58" s="90" t="s">
+        <v>225</v>
+      </c>
+      <c r="D58" s="93" t="s">
+        <v>152</v>
+      </c>
+      <c r="E58" s="93" t="s">
         <v>36</v>
       </c>
-      <c r="F58" s="94" t="s">
-        <v>299</v>
+      <c r="F58" s="93" t="s">
+        <v>298</v>
       </c>
       <c r="G58" s="22" t="s">
         <v>37</v>
@@ -5296,58 +5299,58 @@
       <c r="B59" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C59" s="91" t="s">
-        <v>226</v>
-      </c>
-      <c r="D59" s="94" t="s">
-        <v>153</v>
-      </c>
-      <c r="E59" s="94" t="s">
+      <c r="C59" s="90" t="s">
+        <v>225</v>
+      </c>
+      <c r="D59" s="93" t="s">
+        <v>152</v>
+      </c>
+      <c r="E59" s="93" t="s">
         <v>38</v>
       </c>
-      <c r="F59" s="94" t="s">
-        <v>300</v>
+      <c r="F59" s="93" t="s">
+        <v>299</v>
       </c>
       <c r="G59" s="22" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B60" s="107" t="s">
+      <c r="B60" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="C60" s="110" t="s">
-        <v>226</v>
-      </c>
-      <c r="D60" s="111" t="s">
-        <v>153</v>
-      </c>
-      <c r="E60" s="111" t="s">
+      <c r="C60" s="109" t="s">
+        <v>225</v>
+      </c>
+      <c r="D60" s="110" t="s">
+        <v>152</v>
+      </c>
+      <c r="E60" s="110" t="s">
         <v>40</v>
       </c>
-      <c r="F60" s="111" t="s">
-        <v>301</v>
-      </c>
-      <c r="G60" s="107" t="s">
+      <c r="F60" s="110" t="s">
+        <v>300</v>
+      </c>
+      <c r="G60" s="106" t="s">
         <v>41</v>
       </c>
-      <c r="H60" s="107"/>
+      <c r="H60" s="106"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B61" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C61" s="91" t="s">
-        <v>226</v>
-      </c>
-      <c r="D61" s="97" t="s">
-        <v>154</v>
+      <c r="C61" s="90" t="s">
+        <v>225</v>
+      </c>
+      <c r="D61" s="96" t="s">
+        <v>153</v>
       </c>
       <c r="E61" s="38" t="s">
         <v>42</v>
       </c>
       <c r="F61" s="38" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G61" s="38"/>
       <c r="H61" s="38"/>
@@ -5356,68 +5359,68 @@
       <c r="B62" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C62" s="91" t="s">
-        <v>226</v>
-      </c>
-      <c r="D62" s="97" t="s">
-        <v>154</v>
-      </c>
-      <c r="E62" s="97" t="s">
+      <c r="C62" s="90" t="s">
+        <v>225</v>
+      </c>
+      <c r="D62" s="96" t="s">
+        <v>153</v>
+      </c>
+      <c r="E62" s="96" t="s">
         <v>18</v>
       </c>
-      <c r="F62" s="97" t="s">
-        <v>303</v>
+      <c r="F62" s="96" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B63" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C63" s="91" t="s">
-        <v>226</v>
-      </c>
-      <c r="D63" s="97" t="s">
-        <v>154</v>
-      </c>
-      <c r="E63" s="97" t="s">
+      <c r="C63" s="90" t="s">
+        <v>225</v>
+      </c>
+      <c r="D63" s="96" t="s">
+        <v>153</v>
+      </c>
+      <c r="E63" s="96" t="s">
         <v>19</v>
       </c>
-      <c r="F63" s="97" t="s">
-        <v>304</v>
+      <c r="F63" s="96" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B64" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C64" s="91" t="s">
-        <v>226</v>
-      </c>
-      <c r="D64" s="97" t="s">
-        <v>154</v>
-      </c>
-      <c r="E64" s="97" t="s">
+      <c r="C64" s="90" t="s">
+        <v>225</v>
+      </c>
+      <c r="D64" s="96" t="s">
+        <v>153</v>
+      </c>
+      <c r="E64" s="96" t="s">
         <v>20</v>
       </c>
-      <c r="F64" s="97" t="s">
-        <v>305</v>
+      <c r="F64" s="96" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B65" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C65" s="91" t="s">
-        <v>226</v>
-      </c>
-      <c r="D65" s="97" t="s">
-        <v>154</v>
-      </c>
-      <c r="E65" s="97" t="s">
+      <c r="C65" s="90" t="s">
+        <v>225</v>
+      </c>
+      <c r="D65" s="96" t="s">
+        <v>153</v>
+      </c>
+      <c r="E65" s="96" t="s">
         <v>21</v>
       </c>
-      <c r="F65" s="97" t="s">
-        <v>306</v>
+      <c r="F65" s="96" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
@@ -5425,36 +5428,36 @@
       <c r="B66" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C66" s="104" t="s">
-        <v>226</v>
-      </c>
-      <c r="D66" s="100" t="s">
-        <v>154</v>
-      </c>
-      <c r="E66" s="100" t="s">
+      <c r="C66" s="103" t="s">
+        <v>225</v>
+      </c>
+      <c r="D66" s="99" t="s">
+        <v>153</v>
+      </c>
+      <c r="E66" s="99" t="s">
         <v>22</v>
       </c>
-      <c r="F66" s="100" t="s">
-        <v>307</v>
+      <c r="F66" s="99" t="s">
+        <v>306</v>
       </c>
       <c r="G66" s="23"/>
-      <c r="H66" s="103"/>
+      <c r="H66" s="102"/>
     </row>
     <row r="67" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B67" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="C67" s="91" t="s">
-        <v>226</v>
-      </c>
-      <c r="D67" s="94" t="s">
-        <v>155</v>
+      <c r="C67" s="90" t="s">
+        <v>225</v>
+      </c>
+      <c r="D67" s="93" t="s">
+        <v>154</v>
       </c>
       <c r="E67" s="38" t="s">
         <v>73</v>
       </c>
       <c r="F67" s="38" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G67" s="38"/>
     </row>
@@ -5462,17 +5465,17 @@
       <c r="B68" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="C68" s="91" t="s">
-        <v>226</v>
-      </c>
-      <c r="D68" s="94" t="s">
-        <v>155</v>
-      </c>
-      <c r="E68" s="94" t="s">
+      <c r="C68" s="90" t="s">
+        <v>225</v>
+      </c>
+      <c r="D68" s="93" t="s">
+        <v>154</v>
+      </c>
+      <c r="E68" s="93" t="s">
         <v>51</v>
       </c>
-      <c r="F68" s="94" t="s">
-        <v>310</v>
+      <c r="F68" s="93" t="s">
+        <v>309</v>
       </c>
       <c r="G68" s="22" t="s">
         <v>52</v>
@@ -5482,17 +5485,17 @@
       <c r="B69" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="C69" s="91" t="s">
-        <v>226</v>
-      </c>
-      <c r="D69" s="94" t="s">
-        <v>155</v>
-      </c>
-      <c r="E69" s="94" t="s">
+      <c r="C69" s="90" t="s">
+        <v>225</v>
+      </c>
+      <c r="D69" s="93" t="s">
+        <v>154</v>
+      </c>
+      <c r="E69" s="93" t="s">
         <v>53</v>
       </c>
-      <c r="F69" s="94" t="s">
-        <v>311</v>
+      <c r="F69" s="93" t="s">
+        <v>310</v>
       </c>
       <c r="G69" s="22" t="s">
         <v>54</v>
@@ -5502,75 +5505,75 @@
       <c r="B70" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="C70" s="91" t="s">
-        <v>226</v>
-      </c>
-      <c r="D70" s="94" t="s">
-        <v>155</v>
-      </c>
-      <c r="E70" s="94" t="s">
+      <c r="C70" s="90" t="s">
+        <v>225</v>
+      </c>
+      <c r="D70" s="93" t="s">
+        <v>154</v>
+      </c>
+      <c r="E70" s="93" t="s">
         <v>55</v>
       </c>
-      <c r="F70" s="94" t="s">
-        <v>312</v>
+      <c r="F70" s="93" t="s">
+        <v>311</v>
       </c>
       <c r="G70" s="22" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B71" s="107" t="s">
+      <c r="B71" s="106" t="s">
         <v>94</v>
       </c>
-      <c r="C71" s="110" t="s">
-        <v>226</v>
-      </c>
-      <c r="D71" s="111" t="s">
-        <v>155</v>
-      </c>
-      <c r="E71" s="111" t="s">
+      <c r="C71" s="109" t="s">
+        <v>225</v>
+      </c>
+      <c r="D71" s="110" t="s">
+        <v>154</v>
+      </c>
+      <c r="E71" s="110" t="s">
         <v>57</v>
       </c>
-      <c r="F71" s="111" t="s">
-        <v>313</v>
-      </c>
-      <c r="G71" s="107" t="s">
+      <c r="F71" s="110" t="s">
+        <v>312</v>
+      </c>
+      <c r="G71" s="106" t="s">
         <v>58</v>
       </c>
-      <c r="H71" s="107"/>
+      <c r="H71" s="106"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B72" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="C72" s="91" t="s">
-        <v>226</v>
-      </c>
-      <c r="D72" s="97" t="s">
-        <v>154</v>
+      <c r="C72" s="90" t="s">
+        <v>225</v>
+      </c>
+      <c r="D72" s="96" t="s">
+        <v>153</v>
       </c>
       <c r="E72" s="38" t="s">
         <v>59</v>
       </c>
       <c r="F72" s="38" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B73" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="C73" s="91" t="s">
-        <v>226</v>
-      </c>
-      <c r="D73" s="97" t="s">
-        <v>154</v>
-      </c>
-      <c r="E73" s="97" t="s">
+      <c r="C73" s="90" t="s">
+        <v>225</v>
+      </c>
+      <c r="D73" s="96" t="s">
+        <v>153</v>
+      </c>
+      <c r="E73" s="96" t="s">
         <v>60</v>
       </c>
-      <c r="F73" s="97" t="s">
-        <v>315</v>
+      <c r="F73" s="96" t="s">
+        <v>314</v>
       </c>
       <c r="G73" s="22" t="s">
         <v>61</v>
@@ -5580,228 +5583,228 @@
       <c r="B74" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="C74" s="91" t="s">
-        <v>226</v>
-      </c>
-      <c r="D74" s="97" t="s">
-        <v>154</v>
-      </c>
-      <c r="E74" s="97" t="s">
+      <c r="C74" s="90" t="s">
+        <v>225</v>
+      </c>
+      <c r="D74" s="96" t="s">
+        <v>153</v>
+      </c>
+      <c r="E74" s="96" t="s">
         <v>62</v>
       </c>
-      <c r="F74" s="97" t="s">
-        <v>316</v>
+      <c r="F74" s="96" t="s">
+        <v>315</v>
       </c>
       <c r="G74" s="22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="71"/>
-      <c r="B75" s="71" t="s">
+      <c r="A75" s="70"/>
+      <c r="B75" s="70" t="s">
         <v>94</v>
       </c>
-      <c r="C75" s="91" t="s">
-        <v>226</v>
-      </c>
-      <c r="D75" s="98" t="s">
-        <v>154</v>
-      </c>
-      <c r="E75" s="98" t="s">
+      <c r="C75" s="90" t="s">
+        <v>225</v>
+      </c>
+      <c r="D75" s="97" t="s">
+        <v>153</v>
+      </c>
+      <c r="E75" s="97" t="s">
         <v>64</v>
       </c>
-      <c r="F75" s="98" t="s">
-        <v>314</v>
-      </c>
-      <c r="G75" s="71" t="s">
+      <c r="F75" s="97" t="s">
+        <v>313</v>
+      </c>
+      <c r="G75" s="70" t="s">
         <v>65</v>
       </c>
-      <c r="H75" s="71"/>
+      <c r="H75" s="70"/>
     </row>
     <row r="76" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="102" t="s">
+      <c r="A76" s="101" t="s">
         <v>95</v>
       </c>
       <c r="B76" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="C76" s="91" t="s">
-        <v>226</v>
-      </c>
-      <c r="E76" s="70" t="s">
+      <c r="C76" s="90" t="s">
+        <v>225</v>
+      </c>
+      <c r="E76" s="69" t="s">
         <v>71</v>
       </c>
       <c r="F76" s="38" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B77" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="C77" s="91" t="s">
-        <v>226</v>
-      </c>
-      <c r="D77" s="97" t="s">
-        <v>154</v>
-      </c>
-      <c r="E77" s="68" t="s">
+      <c r="C77" s="90" t="s">
+        <v>225</v>
+      </c>
+      <c r="D77" s="96" t="s">
+        <v>153</v>
+      </c>
+      <c r="E77" s="67" t="s">
         <v>79</v>
       </c>
-      <c r="F77" s="97" t="s">
-        <v>318</v>
+      <c r="F77" s="96" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="B78" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="C78" s="91" t="s">
-        <v>226</v>
-      </c>
-      <c r="E78" s="67" t="s">
+      <c r="C78" s="90" t="s">
+        <v>225</v>
+      </c>
+      <c r="E78" s="66" t="s">
         <v>80</v>
       </c>
       <c r="F78" s="22" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="70"/>
+      <c r="B79" s="70" t="s">
+        <v>85</v>
+      </c>
+      <c r="C79" s="90" t="s">
+        <v>225</v>
+      </c>
+      <c r="D79" s="70"/>
+      <c r="E79" s="72" t="s">
+        <v>81</v>
+      </c>
+      <c r="F79" s="70" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="71"/>
-      <c r="B79" s="71" t="s">
-        <v>85</v>
-      </c>
-      <c r="C79" s="91" t="s">
-        <v>226</v>
-      </c>
-      <c r="D79" s="71"/>
-      <c r="E79" s="73" t="s">
-        <v>81</v>
-      </c>
-      <c r="F79" s="71" t="s">
-        <v>320</v>
-      </c>
-      <c r="G79" s="71"/>
-      <c r="H79" s="71"/>
+      <c r="G79" s="70"/>
+      <c r="H79" s="70"/>
     </row>
     <row r="80" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="102" t="s">
-        <v>231</v>
+      <c r="A80" s="101" t="s">
+        <v>230</v>
       </c>
       <c r="B80" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="C80" s="91" t="s">
-        <v>226</v>
-      </c>
-      <c r="E80" s="76" t="s">
+      <c r="C80" s="90" t="s">
+        <v>225</v>
+      </c>
+      <c r="E80" s="75" t="s">
         <v>71</v>
       </c>
       <c r="F80" s="38" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
       <c r="B81" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="C81" s="91" t="s">
-        <v>226</v>
-      </c>
-      <c r="E81" s="64" t="s">
+      <c r="C81" s="90" t="s">
+        <v>225</v>
+      </c>
+      <c r="E81" s="63" t="s">
+        <v>233</v>
+      </c>
+      <c r="F81" s="22" t="s">
+        <v>321</v>
+      </c>
+      <c r="G81" s="64"/>
+    </row>
+    <row r="82" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A82" s="102"/>
+      <c r="B82" s="102" t="s">
+        <v>85</v>
+      </c>
+      <c r="C82" s="103" t="s">
+        <v>225</v>
+      </c>
+      <c r="D82" s="102"/>
+      <c r="E82" s="111" t="s">
         <v>234</v>
       </c>
-      <c r="F81" s="22" t="s">
+      <c r="F82" s="102" t="s">
         <v>322</v>
       </c>
-      <c r="G81" s="65"/>
-    </row>
-    <row r="82" spans="1:8" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A82" s="103"/>
-      <c r="B82" s="103" t="s">
-        <v>85</v>
-      </c>
-      <c r="C82" s="104" t="s">
-        <v>226</v>
-      </c>
-      <c r="D82" s="103"/>
-      <c r="E82" s="112" t="s">
-        <v>235</v>
-      </c>
-      <c r="F82" s="103" t="s">
-        <v>323</v>
-      </c>
-      <c r="G82" s="113"/>
-      <c r="H82" s="103"/>
+      <c r="G82" s="112"/>
+      <c r="H82" s="102"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B83" s="22" t="s">
+        <v>235</v>
+      </c>
+      <c r="C83" s="90" t="s">
+        <v>225</v>
+      </c>
+      <c r="D83" s="93" t="s">
+        <v>154</v>
+      </c>
+      <c r="E83" s="75" t="s">
         <v>236</v>
       </c>
-      <c r="C83" s="91" t="s">
-        <v>226</v>
-      </c>
-      <c r="D83" s="94" t="s">
-        <v>155</v>
-      </c>
-      <c r="E83" s="76" t="s">
-        <v>237</v>
-      </c>
       <c r="F83" s="38" t="s">
-        <v>324</v>
-      </c>
-      <c r="G83" s="65"/>
+        <v>323</v>
+      </c>
+      <c r="G83" s="64"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B84" s="22" t="s">
-        <v>236</v>
-      </c>
-      <c r="C84" s="91" t="s">
-        <v>226</v>
-      </c>
-      <c r="D84" s="94" t="s">
-        <v>155</v>
-      </c>
-      <c r="E84" s="95" t="s">
+        <v>235</v>
+      </c>
+      <c r="C84" s="90" t="s">
+        <v>225</v>
+      </c>
+      <c r="D84" s="93" t="s">
+        <v>154</v>
+      </c>
+      <c r="E84" s="94" t="s">
+        <v>237</v>
+      </c>
+      <c r="F84" s="93" t="s">
+        <v>324</v>
+      </c>
+      <c r="G84" s="63" t="s">
         <v>238</v>
       </c>
-      <c r="F84" s="94" t="s">
+    </row>
+    <row r="85" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="70"/>
+      <c r="B85" s="70" t="s">
+        <v>235</v>
+      </c>
+      <c r="C85" s="91" t="s">
+        <v>225</v>
+      </c>
+      <c r="D85" s="98" t="s">
+        <v>154</v>
+      </c>
+      <c r="E85" s="95" t="s">
+        <v>239</v>
+      </c>
+      <c r="F85" s="98" t="s">
         <v>325</v>
       </c>
-      <c r="G84" s="64" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="71"/>
-      <c r="B85" s="71" t="s">
-        <v>236</v>
-      </c>
-      <c r="C85" s="92" t="s">
-        <v>226</v>
-      </c>
-      <c r="D85" s="99" t="s">
-        <v>155</v>
-      </c>
-      <c r="E85" s="96" t="s">
+      <c r="G85" s="76" t="s">
         <v>240</v>
       </c>
-      <c r="F85" s="99" t="s">
-        <v>326</v>
-      </c>
-      <c r="G85" s="77" t="s">
-        <v>241</v>
-      </c>
-      <c r="H85" s="71"/>
+      <c r="H85" s="70"/>
     </row>
     <row r="86" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="G86" s="65"/>
+      <c r="G86" s="64"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="G87" s="65"/>
+      <c r="G87" s="64"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A89" s="93"/>
+      <c r="A89" s="92"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5928,10 +5931,10 @@
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="113" t="s">
         <v>86</v>
       </c>
-      <c r="B12" s="39"/>
+      <c r="B12" s="113"/>
       <c r="C12" s="12" t="s">
         <v>32</v>
       </c>
@@ -5992,10 +5995,10 @@
       <c r="D18" s="11"/>
     </row>
     <row r="19" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="39" t="s">
+      <c r="A19" s="113" t="s">
         <v>93</v>
       </c>
-      <c r="B19" s="39"/>
+      <c r="B19" s="113"/>
       <c r="C19" s="10" t="s">
         <v>18</v>
       </c>
@@ -6044,10 +6047,10 @@
       <c r="D24" s="12"/>
     </row>
     <row r="25" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="39" t="s">
+      <c r="A25" s="113" t="s">
         <v>86</v>
       </c>
-      <c r="B25" s="39"/>
+      <c r="B25" s="113"/>
       <c r="C25" s="10" t="s">
         <v>51</v>
       </c>
@@ -6094,10 +6097,10 @@
       <c r="D29" s="6"/>
     </row>
     <row r="30" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="113" t="s">
         <v>93</v>
       </c>
-      <c r="B30" s="39"/>
+      <c r="B30" s="113"/>
       <c r="C30" s="12" t="s">
         <v>60</v>
       </c>
@@ -6196,12 +6199,12 @@
     </row>
     <row r="41" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C41" s="60" t="s">
+      <c r="C41" s="59" t="s">
         <v>70</v>
       </c>
       <c r="D41" s="17"/>
@@ -6218,7 +6221,7 @@
       <c r="A43" s="18"/>
       <c r="B43" s="18"/>
       <c r="C43" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D43" s="2"/>
     </row>
@@ -6226,7 +6229,7 @@
       <c r="A44" s="18"/>
       <c r="B44" s="18"/>
       <c r="C44" s="12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D44" s="12"/>
     </row>
@@ -6244,7 +6247,7 @@
       <c r="A46" s="18"/>
       <c r="B46" s="18"/>
       <c r="C46" s="12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D46" s="12"/>
     </row>
@@ -6252,17 +6255,17 @@
       <c r="A47" s="18"/>
       <c r="B47" s="18"/>
       <c r="C47" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D47" s="2"/>
     </row>
     <row r="48" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="18"/>
       <c r="B48" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="C48" s="12" t="s">
         <v>236</v>
-      </c>
-      <c r="C48" s="12" t="s">
-        <v>237</v>
       </c>
       <c r="D48" s="12"/>
     </row>
@@ -6270,20 +6273,20 @@
       <c r="A49" s="18"/>
       <c r="B49" s="18"/>
       <c r="C49" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="D49" s="10" t="s">
         <v>238</v>
-      </c>
-      <c r="D49" s="10" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="D50" s="9" t="s">
         <v>240</v>
-      </c>
-      <c r="D50" s="9" t="s">
-        <v>241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>